<commit_message>
1st run MMLR including Free tram zone
</commit_message>
<xml_diff>
--- a/BE-TR_Co-Located_stops.xlsx
+++ b/BE-TR_Co-Located_stops.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lkast1\Google Drive\PhD\2.Analysis\2. Empirical Analysis\BE-TR_Multi Country Samples\Melbourne\Melb.All.Stops\Melb.AllStops.Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E8C5EF9-6BD4-4AFC-9CA3-FAC2D8C0089B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D030C09-75A3-4F33-888D-7C6F06A66CAE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="4730" windowHeight="2790" xr2:uid="{B50390F9-1CAC-4F81-963B-4903969F49F6}"/>
   </bookViews>
@@ -16,6 +16,10 @@
     <sheet name="Tram-bus-overlap-160" sheetId="2" r:id="rId1"/>
     <sheet name="Train-bus-overlap-160" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Train-bus-overlap-160'!$A$1:$AB$192</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tram-bus-overlap-160'!$A$1:$AB$469</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -3415,11 +3419,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1809AB1F-5609-4A5B-8B17-BC50163CBDBD}">
   <dimension ref="A1:AB469"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2:AB469"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB1" sqref="AB1:AB1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -3584,7 +3591,7 @@
         <v>5802444.5153999999</v>
       </c>
       <c r="AB2">
-        <v>5.8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.35">
@@ -3664,7 +3671,7 @@
         <v>5802710.5088999998</v>
       </c>
       <c r="AB3">
-        <v>4.9000000000000004</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.35">
@@ -3984,7 +3991,7 @@
         <v>5804023.0036000004</v>
       </c>
       <c r="AB7">
-        <v>3.4</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.35">
@@ -4224,7 +4231,7 @@
         <v>5805051.6851000004</v>
       </c>
       <c r="AB10">
-        <v>10.9</v>
+        <v>214.1</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.35">
@@ -4304,7 +4311,7 @@
         <v>5805059.4874999998</v>
       </c>
       <c r="AB11">
-        <v>1.9</v>
+        <v>7.1999999999999993</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.35">
@@ -4384,7 +4391,7 @@
         <v>5805081.6752000004</v>
       </c>
       <c r="AB12">
-        <v>32.700000000000003</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.35">
@@ -4784,7 +4791,7 @@
         <v>5805191.5027000001</v>
       </c>
       <c r="AB17">
-        <v>18.3</v>
+        <v>24.1</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.35">
@@ -4864,7 +4871,7 @@
         <v>5805191.5027000001</v>
       </c>
       <c r="AB18">
-        <v>18.3</v>
+        <v>24.1</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.35">
@@ -5024,7 +5031,7 @@
         <v>5805656.4916000003</v>
       </c>
       <c r="AB20">
-        <v>5.9</v>
+        <v>25.299999999999997</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.35">
@@ -5104,7 +5111,7 @@
         <v>5805989.5020000003</v>
       </c>
       <c r="AB21">
-        <v>1.4</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.35">
@@ -5184,7 +5191,7 @@
         <v>5805995.0094999997</v>
       </c>
       <c r="AB22">
-        <v>8</v>
+        <v>1099.3999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.35">
@@ -5264,7 +5271,7 @@
         <v>5806061.0335999997</v>
       </c>
       <c r="AB23">
-        <v>0.9</v>
+        <v>5.3000000000000007</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.35">
@@ -5344,7 +5351,7 @@
         <v>5806061.0335999997</v>
       </c>
       <c r="AB24">
-        <v>0.9</v>
+        <v>5.3000000000000007</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.35">
@@ -5424,7 +5431,7 @@
         <v>5806132.9764</v>
       </c>
       <c r="AB25">
-        <v>0.3</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.35">
@@ -5984,7 +5991,7 @@
         <v>5806604.6550000003</v>
       </c>
       <c r="AB32">
-        <v>5</v>
+        <v>16.600000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.35">
@@ -6224,7 +6231,7 @@
         <v>5806683.0042000003</v>
       </c>
       <c r="AB35">
-        <v>14.1</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.35">
@@ -6304,7 +6311,7 @@
         <v>5806762.4862000002</v>
       </c>
       <c r="AB36">
-        <v>169.9</v>
+        <v>265.5</v>
       </c>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.35">
@@ -6384,7 +6391,7 @@
         <v>5806781.9985999996</v>
       </c>
       <c r="AB37">
-        <v>12.3</v>
+        <v>18.600000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.35">
@@ -6624,7 +6631,7 @@
         <v>5807005.0066</v>
       </c>
       <c r="AB40">
-        <v>13.8</v>
+        <v>84.3</v>
       </c>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.35">
@@ -6704,7 +6711,7 @@
         <v>5807005.0066</v>
       </c>
       <c r="AB41">
-        <v>13.8</v>
+        <v>84.3</v>
       </c>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.35">
@@ -6944,7 +6951,7 @@
         <v>5807013.9762000004</v>
       </c>
       <c r="AB44">
-        <v>0.4</v>
+        <v>96.1</v>
       </c>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.35">
@@ -7344,7 +7351,7 @@
         <v>5807347.0153000001</v>
       </c>
       <c r="AB49">
-        <v>2.2999999999999998</v>
+        <v>4.1999999999999993</v>
       </c>
     </row>
     <row r="50" spans="1:28" x14ac:dyDescent="0.35">
@@ -7504,7 +7511,7 @@
         <v>5807501.4837999996</v>
       </c>
       <c r="AB51">
-        <v>8.6999999999999993</v>
+        <v>18.600000000000001</v>
       </c>
     </row>
     <row r="52" spans="1:28" x14ac:dyDescent="0.35">
@@ -7584,7 +7591,7 @@
         <v>5807664.4903999995</v>
       </c>
       <c r="AB52">
-        <v>17.2</v>
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="53" spans="1:28" x14ac:dyDescent="0.35">
@@ -7664,7 +7671,7 @@
         <v>5807664.4903999995</v>
       </c>
       <c r="AB53">
-        <v>17.2</v>
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.35">
@@ -7744,7 +7751,7 @@
         <v>5807664.4903999995</v>
       </c>
       <c r="AB54">
-        <v>17.2</v>
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="55" spans="1:28" x14ac:dyDescent="0.35">
@@ -7824,7 +7831,7 @@
         <v>5807693.0135000004</v>
       </c>
       <c r="AB55">
-        <v>1.1000000000000001</v>
+        <v>10.299999999999999</v>
       </c>
     </row>
     <row r="56" spans="1:28" x14ac:dyDescent="0.35">
@@ -7904,7 +7911,7 @@
         <v>5807693.0135000004</v>
       </c>
       <c r="AB56">
-        <v>1.1000000000000001</v>
+        <v>10.299999999999999</v>
       </c>
     </row>
     <row r="57" spans="1:28" x14ac:dyDescent="0.35">
@@ -8064,7 +8071,7 @@
         <v>5807874.4689999996</v>
       </c>
       <c r="AB58">
-        <v>0.7</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="59" spans="1:28" x14ac:dyDescent="0.35">
@@ -8464,7 +8471,7 @@
         <v>5808027.4797</v>
       </c>
       <c r="AB63">
-        <v>26.9</v>
+        <v>52</v>
       </c>
     </row>
     <row r="64" spans="1:28" x14ac:dyDescent="0.35">
@@ -8544,7 +8551,7 @@
         <v>5808027.4797</v>
       </c>
       <c r="AB64">
-        <v>26.9</v>
+        <v>52</v>
       </c>
     </row>
     <row r="65" spans="1:28" x14ac:dyDescent="0.35">
@@ -8624,7 +8631,7 @@
         <v>5808068.966</v>
       </c>
       <c r="AB65">
-        <v>4.0999999999999996</v>
+        <v>5.8999999999999995</v>
       </c>
     </row>
     <row r="66" spans="1:28" x14ac:dyDescent="0.35">
@@ -8704,7 +8711,7 @@
         <v>5808116.5066</v>
       </c>
       <c r="AB66">
-        <v>12.1</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="67" spans="1:28" x14ac:dyDescent="0.35">
@@ -8944,7 +8951,7 @@
         <v>5808277.5170999998</v>
       </c>
       <c r="AB69">
-        <v>0.2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="70" spans="1:28" x14ac:dyDescent="0.35">
@@ -9104,7 +9111,7 @@
         <v>5808364.4950000001</v>
       </c>
       <c r="AB71">
-        <v>6.3</v>
+        <v>22.2</v>
       </c>
     </row>
     <row r="72" spans="1:28" x14ac:dyDescent="0.35">
@@ -9184,7 +9191,7 @@
         <v>5808487.0443000002</v>
       </c>
       <c r="AB72">
-        <v>5.6</v>
+        <v>17.100000000000001</v>
       </c>
     </row>
     <row r="73" spans="1:28" x14ac:dyDescent="0.35">
@@ -9264,7 +9271,7 @@
         <v>5808504.7887000004</v>
       </c>
       <c r="AB73">
-        <v>2.4</v>
+        <v>207.3</v>
       </c>
     </row>
     <row r="74" spans="1:28" x14ac:dyDescent="0.35">
@@ -9344,7 +9351,7 @@
         <v>5808527.5395999998</v>
       </c>
       <c r="AB74">
-        <v>0.4</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="75" spans="1:28" x14ac:dyDescent="0.35">
@@ -9424,7 +9431,7 @@
         <v>5808566.5091000004</v>
       </c>
       <c r="AB75">
-        <v>7.6</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="76" spans="1:28" x14ac:dyDescent="0.35">
@@ -9664,7 +9671,7 @@
         <v>5808670.0261000004</v>
       </c>
       <c r="AB78">
-        <v>4.9000000000000004</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="79" spans="1:28" x14ac:dyDescent="0.35">
@@ -9904,7 +9911,7 @@
         <v>5808793.5278000003</v>
       </c>
       <c r="AB81">
-        <v>87.9</v>
+        <v>212.7</v>
       </c>
     </row>
     <row r="82" spans="1:28" x14ac:dyDescent="0.35">
@@ -9984,7 +9991,7 @@
         <v>5808793.5278000003</v>
       </c>
       <c r="AB82">
-        <v>87.9</v>
+        <v>212.7</v>
       </c>
     </row>
     <row r="83" spans="1:28" x14ac:dyDescent="0.35">
@@ -10144,7 +10151,7 @@
         <v>5808813.0144999996</v>
       </c>
       <c r="AB84">
-        <v>1.5</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="85" spans="1:28" x14ac:dyDescent="0.35">
@@ -10224,7 +10231,7 @@
         <v>5808816.9993000003</v>
       </c>
       <c r="AB85">
-        <v>12.7</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="86" spans="1:28" x14ac:dyDescent="0.35">
@@ -10304,7 +10311,7 @@
         <v>5808846.0347999996</v>
       </c>
       <c r="AB86">
-        <v>40.9</v>
+        <v>64.400000000000006</v>
       </c>
     </row>
     <row r="87" spans="1:28" x14ac:dyDescent="0.35">
@@ -10384,7 +10391,7 @@
         <v>5808850.5093</v>
       </c>
       <c r="AB87">
-        <v>2.2999999999999998</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88" spans="1:28" x14ac:dyDescent="0.35">
@@ -10464,7 +10471,7 @@
         <v>5808909.9967999998</v>
       </c>
       <c r="AB88">
-        <v>6.9</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="89" spans="1:28" x14ac:dyDescent="0.35">
@@ -10544,7 +10551,7 @@
         <v>5808915.0140000004</v>
       </c>
       <c r="AB89">
-        <v>151.30000000000001</v>
+        <v>245.90000000000003</v>
       </c>
     </row>
     <row r="90" spans="1:28" x14ac:dyDescent="0.35">
@@ -10624,7 +10631,7 @@
         <v>5808915.0140000004</v>
       </c>
       <c r="AB90">
-        <v>151.30000000000001</v>
+        <v>245.90000000000003</v>
       </c>
     </row>
     <row r="91" spans="1:28" x14ac:dyDescent="0.35">
@@ -10944,7 +10951,7 @@
         <v>5808998.0005999999</v>
       </c>
       <c r="AB94">
-        <v>18.899999999999999</v>
+        <v>193.7</v>
       </c>
     </row>
     <row r="95" spans="1:28" x14ac:dyDescent="0.35">
@@ -11024,7 +11031,7 @@
         <v>5808999.0296</v>
       </c>
       <c r="AB95">
-        <v>23.3</v>
+        <v>29.3</v>
       </c>
     </row>
     <row r="96" spans="1:28" x14ac:dyDescent="0.35">
@@ -11104,7 +11111,7 @@
         <v>5809021.0261000004</v>
       </c>
       <c r="AB96">
-        <v>73.900000000000006</v>
+        <v>255.70000000000002</v>
       </c>
     </row>
     <row r="97" spans="1:28" x14ac:dyDescent="0.35">
@@ -11184,7 +11191,7 @@
         <v>5809032.9945</v>
       </c>
       <c r="AB97">
-        <v>21.4</v>
+        <v>27.7</v>
       </c>
     </row>
     <row r="98" spans="1:28" x14ac:dyDescent="0.35">
@@ -11264,7 +11271,7 @@
         <v>5809035.2896999996</v>
       </c>
       <c r="AB98">
-        <v>8.6999999999999993</v>
+        <v>24.299999999999997</v>
       </c>
     </row>
     <row r="99" spans="1:28" x14ac:dyDescent="0.35">
@@ -11424,7 +11431,7 @@
         <v>5809058.0115</v>
       </c>
       <c r="AB100">
-        <v>7.3</v>
+        <v>10.3</v>
       </c>
     </row>
     <row r="101" spans="1:28" x14ac:dyDescent="0.35">
@@ -11504,7 +11511,7 @@
         <v>5809060.21</v>
       </c>
       <c r="AB101">
-        <v>2.7</v>
+        <v>42.7</v>
       </c>
     </row>
     <row r="102" spans="1:28" x14ac:dyDescent="0.35">
@@ -11584,7 +11591,7 @@
         <v>5809078.5253999997</v>
       </c>
       <c r="AB102">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="103" spans="1:28" x14ac:dyDescent="0.35">
@@ -11664,7 +11671,7 @@
         <v>5809078.9737999998</v>
       </c>
       <c r="AB103">
-        <v>8.4</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="104" spans="1:28" x14ac:dyDescent="0.35">
@@ -11744,7 +11751,7 @@
         <v>5809078.9737999998</v>
       </c>
       <c r="AB104">
-        <v>8.4</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="105" spans="1:28" x14ac:dyDescent="0.35">
@@ -11824,7 +11831,7 @@
         <v>5809089.7545999996</v>
       </c>
       <c r="AB105">
-        <v>58.1</v>
+        <v>205.3</v>
       </c>
     </row>
     <row r="106" spans="1:28" x14ac:dyDescent="0.35">
@@ -11904,7 +11911,7 @@
         <v>5809089.7545999996</v>
       </c>
       <c r="AB106">
-        <v>58.1</v>
+        <v>205.3</v>
       </c>
     </row>
     <row r="107" spans="1:28" x14ac:dyDescent="0.35">
@@ -11984,7 +11991,7 @@
         <v>5809119.9944000002</v>
       </c>
       <c r="AB107">
-        <v>7.7</v>
+        <v>14.9</v>
       </c>
     </row>
     <row r="108" spans="1:28" x14ac:dyDescent="0.35">
@@ -12064,7 +12071,7 @@
         <v>5809138.7631000001</v>
       </c>
       <c r="AB108">
-        <v>10.1</v>
+        <v>30.9</v>
       </c>
     </row>
     <row r="109" spans="1:28" x14ac:dyDescent="0.35">
@@ -12144,7 +12151,7 @@
         <v>5809145.5392000005</v>
       </c>
       <c r="AB109">
-        <v>64.3</v>
+        <v>208.89999999999998</v>
       </c>
     </row>
     <row r="110" spans="1:28" x14ac:dyDescent="0.35">
@@ -12224,7 +12231,7 @@
         <v>5809154.5016000001</v>
       </c>
       <c r="AB110">
-        <v>2.6</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="111" spans="1:28" x14ac:dyDescent="0.35">
@@ -12304,7 +12311,7 @@
         <v>5809198.4914999995</v>
       </c>
       <c r="AB111">
-        <v>9.1</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="112" spans="1:28" x14ac:dyDescent="0.35">
@@ -12384,7 +12391,7 @@
         <v>5809198.4914999995</v>
       </c>
       <c r="AB112">
-        <v>9.1</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="113" spans="1:28" x14ac:dyDescent="0.35">
@@ -12464,7 +12471,7 @@
         <v>5809228.4736000001</v>
       </c>
       <c r="AB113">
-        <v>18.2</v>
+        <v>36.700000000000003</v>
       </c>
     </row>
     <row r="114" spans="1:28" x14ac:dyDescent="0.35">
@@ -12544,7 +12551,7 @@
         <v>5809260.0018999996</v>
       </c>
       <c r="AB114">
-        <v>26.6</v>
+        <v>131.19999999999999</v>
       </c>
     </row>
     <row r="115" spans="1:28" x14ac:dyDescent="0.35">
@@ -12624,7 +12631,7 @@
         <v>5809291.7123999996</v>
       </c>
       <c r="AB115">
-        <v>49.7</v>
+        <v>207.89999999999998</v>
       </c>
     </row>
     <row r="116" spans="1:28" x14ac:dyDescent="0.35">
@@ -12704,7 +12711,7 @@
         <v>5809291.7123999996</v>
       </c>
       <c r="AB116">
-        <v>49.7</v>
+        <v>207.89999999999998</v>
       </c>
     </row>
     <row r="117" spans="1:28" x14ac:dyDescent="0.35">
@@ -12784,7 +12791,7 @@
         <v>5809367.9952999996</v>
       </c>
       <c r="AB117">
-        <v>8.4</v>
+        <v>27.299999999999997</v>
       </c>
     </row>
     <row r="118" spans="1:28" x14ac:dyDescent="0.35">
@@ -12864,7 +12871,7 @@
         <v>5809377.9851000002</v>
       </c>
       <c r="AB118">
-        <v>175.4</v>
+        <v>236.10000000000002</v>
       </c>
     </row>
     <row r="119" spans="1:28" x14ac:dyDescent="0.35">
@@ -12944,7 +12951,7 @@
         <v>5809431.5171999997</v>
       </c>
       <c r="AB119">
-        <v>5.5</v>
+        <v>29.3</v>
       </c>
     </row>
     <row r="120" spans="1:28" x14ac:dyDescent="0.35">
@@ -13024,7 +13031,7 @@
         <v>5809533.5016999999</v>
       </c>
       <c r="AB120">
-        <v>3.4</v>
+        <v>6.6999999999999993</v>
       </c>
     </row>
     <row r="121" spans="1:28" x14ac:dyDescent="0.35">
@@ -13104,7 +13111,7 @@
         <v>5809865.5327000003</v>
       </c>
       <c r="AB121">
-        <v>3</v>
+        <v>8.1999999999999993</v>
       </c>
     </row>
     <row r="122" spans="1:28" x14ac:dyDescent="0.35">
@@ -13184,7 +13191,7 @@
         <v>5809884.0082999999</v>
       </c>
       <c r="AB122">
-        <v>0.2</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="123" spans="1:28" x14ac:dyDescent="0.35">
@@ -13264,7 +13271,7 @@
         <v>5809953.5125000002</v>
       </c>
       <c r="AB123">
-        <v>9.5</v>
+        <v>23.2</v>
       </c>
     </row>
     <row r="124" spans="1:28" x14ac:dyDescent="0.35">
@@ -13344,7 +13351,7 @@
         <v>5810216.9985999996</v>
       </c>
       <c r="AB124">
-        <v>48.8</v>
+        <v>94</v>
       </c>
     </row>
     <row r="125" spans="1:28" x14ac:dyDescent="0.35">
@@ -13424,7 +13431,7 @@
         <v>5810424.9999000002</v>
       </c>
       <c r="AB125">
-        <v>5.6</v>
+        <v>12.8</v>
       </c>
     </row>
     <row r="126" spans="1:28" x14ac:dyDescent="0.35">
@@ -13504,7 +13511,7 @@
         <v>5810511.9917000001</v>
       </c>
       <c r="AB126">
-        <v>23.8</v>
+        <v>136.1</v>
       </c>
     </row>
     <row r="127" spans="1:28" x14ac:dyDescent="0.35">
@@ -13584,7 +13591,7 @@
         <v>5810564.983</v>
       </c>
       <c r="AB127">
-        <v>4.7</v>
+        <v>13.8</v>
       </c>
     </row>
     <row r="128" spans="1:28" x14ac:dyDescent="0.35">
@@ -13664,7 +13671,7 @@
         <v>5810586.4949000003</v>
       </c>
       <c r="AB128">
-        <v>5.3</v>
+        <v>10.399999999999999</v>
       </c>
     </row>
     <row r="129" spans="1:28" x14ac:dyDescent="0.35">
@@ -13744,7 +13751,7 @@
         <v>5810607.9764</v>
       </c>
       <c r="AB129">
-        <v>1</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="130" spans="1:28" x14ac:dyDescent="0.35">
@@ -13824,7 +13831,7 @@
         <v>5810613.5121999998</v>
       </c>
       <c r="AB130">
-        <v>5.2</v>
+        <v>13.899999999999999</v>
       </c>
     </row>
     <row r="131" spans="1:28" x14ac:dyDescent="0.35">
@@ -13904,7 +13911,7 @@
         <v>5810626.0061999997</v>
       </c>
       <c r="AB131">
-        <v>5.9</v>
+        <v>12.9</v>
       </c>
     </row>
     <row r="132" spans="1:28" x14ac:dyDescent="0.35">
@@ -13984,7 +13991,7 @@
         <v>5810626.0061999997</v>
       </c>
       <c r="AB132">
-        <v>5.9</v>
+        <v>12.9</v>
       </c>
     </row>
     <row r="133" spans="1:28" x14ac:dyDescent="0.35">
@@ -14064,7 +14071,7 @@
         <v>5810646.4779000003</v>
       </c>
       <c r="AB133">
-        <v>2.8</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="134" spans="1:28" x14ac:dyDescent="0.35">
@@ -14144,7 +14151,7 @@
         <v>5810646.4779000003</v>
       </c>
       <c r="AB134">
-        <v>2.8</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="135" spans="1:28" x14ac:dyDescent="0.35">
@@ -14224,7 +14231,7 @@
         <v>5810646.4779000003</v>
       </c>
       <c r="AB135">
-        <v>2.8</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="136" spans="1:28" x14ac:dyDescent="0.35">
@@ -14304,7 +14311,7 @@
         <v>5810655.0356999999</v>
       </c>
       <c r="AB136">
-        <v>6.8</v>
+        <v>20.6</v>
       </c>
     </row>
     <row r="137" spans="1:28" x14ac:dyDescent="0.35">
@@ -14544,7 +14551,7 @@
         <v>5810744.5131000001</v>
       </c>
       <c r="AB139">
-        <v>0.6</v>
+        <v>6.1999999999999993</v>
       </c>
     </row>
     <row r="140" spans="1:28" x14ac:dyDescent="0.35">
@@ -14624,7 +14631,7 @@
         <v>5810837.9937000005</v>
       </c>
       <c r="AB140">
-        <v>3.9</v>
+        <v>12.9</v>
       </c>
     </row>
     <row r="141" spans="1:28" x14ac:dyDescent="0.35">
@@ -14704,7 +14711,7 @@
         <v>5810837.9937000005</v>
       </c>
       <c r="AB141">
-        <v>3.9</v>
+        <v>12.9</v>
       </c>
     </row>
     <row r="142" spans="1:28" x14ac:dyDescent="0.35">
@@ -14944,7 +14951,7 @@
         <v>5811056.9663000004</v>
       </c>
       <c r="AB144">
-        <v>18</v>
+        <v>30.6</v>
       </c>
     </row>
     <row r="145" spans="1:28" x14ac:dyDescent="0.35">
@@ -15024,7 +15031,7 @@
         <v>5811131.5131999999</v>
       </c>
       <c r="AB145">
-        <v>11.8</v>
+        <v>25.1</v>
       </c>
     </row>
     <row r="146" spans="1:28" x14ac:dyDescent="0.35">
@@ -15104,7 +15111,7 @@
         <v>5811143.4660999998</v>
       </c>
       <c r="AB146">
-        <v>4.2</v>
+        <v>36.800000000000004</v>
       </c>
     </row>
     <row r="147" spans="1:28" x14ac:dyDescent="0.35">
@@ -15184,7 +15191,7 @@
         <v>5811143.4660999998</v>
       </c>
       <c r="AB147">
-        <v>4.2</v>
+        <v>36.800000000000004</v>
       </c>
     </row>
     <row r="148" spans="1:28" x14ac:dyDescent="0.35">
@@ -15264,7 +15271,7 @@
         <v>5811264.4880999997</v>
       </c>
       <c r="AB148">
-        <v>10.199999999999999</v>
+        <v>32.4</v>
       </c>
     </row>
     <row r="149" spans="1:28" x14ac:dyDescent="0.35">
@@ -15344,7 +15351,7 @@
         <v>5811283.4848999996</v>
       </c>
       <c r="AB149">
-        <v>32.1</v>
+        <v>50.5</v>
       </c>
     </row>
     <row r="150" spans="1:28" x14ac:dyDescent="0.35">
@@ -15424,7 +15431,7 @@
         <v>5811283.4848999996</v>
       </c>
       <c r="AB150">
-        <v>32.1</v>
+        <v>50.5</v>
       </c>
     </row>
     <row r="151" spans="1:28" x14ac:dyDescent="0.35">
@@ -15504,7 +15511,7 @@
         <v>5811553.4978999998</v>
       </c>
       <c r="AB151">
-        <v>26.8</v>
+        <v>74.8</v>
       </c>
     </row>
     <row r="152" spans="1:28" x14ac:dyDescent="0.35">
@@ -15823,8 +15830,8 @@
       <c r="AA155">
         <v>5812122.9918999998</v>
       </c>
-      <c r="AB155" t="e">
-        <v>#N/A</v>
+      <c r="AB155">
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:28" x14ac:dyDescent="0.35">
@@ -15903,8 +15910,8 @@
       <c r="AA156">
         <v>5812122.9918999998</v>
       </c>
-      <c r="AB156" t="e">
-        <v>#N/A</v>
+      <c r="AB156">
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:28" x14ac:dyDescent="0.35">
@@ -16144,7 +16151,7 @@
         <v>5812267.9834000003</v>
       </c>
       <c r="AB159">
-        <v>882.5</v>
+        <v>900.5</v>
       </c>
     </row>
     <row r="160" spans="1:28" x14ac:dyDescent="0.35">
@@ -16224,7 +16231,7 @@
         <v>5812267.9834000003</v>
       </c>
       <c r="AB160">
-        <v>882.5</v>
+        <v>900.5</v>
       </c>
     </row>
     <row r="161" spans="1:28" x14ac:dyDescent="0.35">
@@ -16304,7 +16311,7 @@
         <v>5812267.9834000003</v>
       </c>
       <c r="AB161">
-        <v>882.5</v>
+        <v>900.5</v>
       </c>
     </row>
     <row r="162" spans="1:28" x14ac:dyDescent="0.35">
@@ -16384,7 +16391,7 @@
         <v>5812346.1765999999</v>
       </c>
       <c r="AB162">
-        <v>11.1</v>
+        <v>397.8</v>
       </c>
     </row>
     <row r="163" spans="1:28" x14ac:dyDescent="0.35">
@@ -16464,7 +16471,7 @@
         <v>5812346.1765999999</v>
       </c>
       <c r="AB163">
-        <v>11.1</v>
+        <v>397.8</v>
       </c>
     </row>
     <row r="164" spans="1:28" x14ac:dyDescent="0.35">
@@ -16544,7 +16551,7 @@
         <v>5812563.0056999996</v>
       </c>
       <c r="AB164">
-        <v>95.6</v>
+        <v>129.39999999999998</v>
       </c>
     </row>
     <row r="165" spans="1:28" x14ac:dyDescent="0.35">
@@ -16624,7 +16631,7 @@
         <v>5812563.0056999996</v>
       </c>
       <c r="AB165">
-        <v>95.6</v>
+        <v>129.39999999999998</v>
       </c>
     </row>
     <row r="166" spans="1:28" x14ac:dyDescent="0.35">
@@ -16704,7 +16711,7 @@
         <v>5812739.5040999996</v>
       </c>
       <c r="AB166">
-        <v>2.9</v>
+        <v>88.7</v>
       </c>
     </row>
     <row r="167" spans="1:28" x14ac:dyDescent="0.35">
@@ -16784,7 +16791,7 @@
         <v>5812767.9807000002</v>
       </c>
       <c r="AB167">
-        <v>38.4</v>
+        <v>188.1</v>
       </c>
     </row>
     <row r="168" spans="1:28" x14ac:dyDescent="0.35">
@@ -16864,7 +16871,7 @@
         <v>5812798.5324999997</v>
       </c>
       <c r="AB168">
-        <v>63</v>
+        <v>83.3</v>
       </c>
     </row>
     <row r="169" spans="1:28" x14ac:dyDescent="0.35">
@@ -16944,7 +16951,7 @@
         <v>5812798.5324999997</v>
       </c>
       <c r="AB169">
-        <v>63</v>
+        <v>83.3</v>
       </c>
     </row>
     <row r="170" spans="1:28" x14ac:dyDescent="0.35">
@@ -17024,7 +17031,7 @@
         <v>5812809.5158000002</v>
       </c>
       <c r="AB170">
-        <v>92.1</v>
+        <v>96.5</v>
       </c>
     </row>
     <row r="171" spans="1:28" x14ac:dyDescent="0.35">
@@ -17104,7 +17111,7 @@
         <v>5812809.5158000002</v>
       </c>
       <c r="AB171">
-        <v>92.1</v>
+        <v>96.5</v>
       </c>
     </row>
     <row r="172" spans="1:28" x14ac:dyDescent="0.35">
@@ -17184,7 +17191,7 @@
         <v>5812839.4685000004</v>
       </c>
       <c r="AB172">
-        <v>47.9</v>
+        <v>2375.1999999999998</v>
       </c>
     </row>
     <row r="173" spans="1:28" x14ac:dyDescent="0.35">
@@ -17264,7 +17271,7 @@
         <v>5812864.983</v>
       </c>
       <c r="AB173">
-        <v>1.2</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="174" spans="1:28" x14ac:dyDescent="0.35">
@@ -17344,7 +17351,7 @@
         <v>5812920.9667999996</v>
       </c>
       <c r="AB174">
-        <v>25.1</v>
+        <v>1067.3</v>
       </c>
     </row>
     <row r="175" spans="1:28" x14ac:dyDescent="0.35">
@@ -17824,7 +17831,7 @@
         <v>5813049.0000999998</v>
       </c>
       <c r="AB180">
-        <v>10.199999999999999</v>
+        <v>28.9</v>
       </c>
     </row>
     <row r="181" spans="1:28" x14ac:dyDescent="0.35">
@@ -17904,7 +17911,7 @@
         <v>5813153.7225000001</v>
       </c>
       <c r="AB181">
-        <v>627.4</v>
+        <v>3258.6000000000004</v>
       </c>
     </row>
     <row r="182" spans="1:28" x14ac:dyDescent="0.35">
@@ -17984,7 +17991,7 @@
         <v>5813182.0195000004</v>
       </c>
       <c r="AB182">
-        <v>27.8</v>
+        <v>39.5</v>
       </c>
     </row>
     <row r="183" spans="1:28" x14ac:dyDescent="0.35">
@@ -18224,7 +18231,7 @@
         <v>5813255.9800000004</v>
       </c>
       <c r="AB185">
-        <v>122.1</v>
+        <v>143</v>
       </c>
     </row>
     <row r="186" spans="1:28" x14ac:dyDescent="0.35">
@@ -18304,7 +18311,7 @@
         <v>5813314.5256000003</v>
       </c>
       <c r="AB186">
-        <v>11.6</v>
+        <v>115.8</v>
       </c>
     </row>
     <row r="187" spans="1:28" x14ac:dyDescent="0.35">
@@ -18384,7 +18391,7 @@
         <v>5813314.5256000003</v>
       </c>
       <c r="AB187">
-        <v>11.6</v>
+        <v>115.8</v>
       </c>
     </row>
     <row r="188" spans="1:28" x14ac:dyDescent="0.35">
@@ -18464,7 +18471,7 @@
         <v>5813362.5033999998</v>
       </c>
       <c r="AB188">
-        <v>101.1</v>
+        <v>104.3</v>
       </c>
     </row>
     <row r="189" spans="1:28" x14ac:dyDescent="0.35">
@@ -18624,7 +18631,7 @@
         <v>5813398.9894000003</v>
       </c>
       <c r="AB190">
-        <v>73.5</v>
+        <v>201.1</v>
       </c>
     </row>
     <row r="191" spans="1:28" x14ac:dyDescent="0.35">
@@ -19504,7 +19511,7 @@
         <v>5813513.0160999997</v>
       </c>
       <c r="AB201">
-        <v>19.8</v>
+        <v>20.2</v>
       </c>
     </row>
     <row r="202" spans="1:28" x14ac:dyDescent="0.35">
@@ -19984,7 +19991,7 @@
         <v>5813547.6688000001</v>
       </c>
       <c r="AB207">
-        <v>39.299999999999997</v>
+        <v>46.3</v>
       </c>
     </row>
     <row r="208" spans="1:28" x14ac:dyDescent="0.35">
@@ -20544,7 +20551,7 @@
         <v>5813665.9808</v>
       </c>
       <c r="AB214">
-        <v>46.6</v>
+        <v>47.1</v>
       </c>
     </row>
     <row r="215" spans="1:28" x14ac:dyDescent="0.35">
@@ -20624,7 +20631,7 @@
         <v>5813665.9808</v>
       </c>
       <c r="AB215">
-        <v>46.6</v>
+        <v>47.1</v>
       </c>
     </row>
     <row r="216" spans="1:28" x14ac:dyDescent="0.35">
@@ -20784,7 +20791,7 @@
         <v>5813746.5367999999</v>
       </c>
       <c r="AB217">
-        <v>273.7</v>
+        <v>373.4</v>
       </c>
     </row>
     <row r="218" spans="1:28" x14ac:dyDescent="0.35">
@@ -21024,7 +21031,7 @@
         <v>5814175.4897999996</v>
       </c>
       <c r="AB220">
-        <v>393.9</v>
+        <v>2846.7</v>
       </c>
     </row>
     <row r="221" spans="1:28" x14ac:dyDescent="0.35">
@@ -21104,7 +21111,7 @@
         <v>5814175.4897999996</v>
       </c>
       <c r="AB221">
-        <v>393.9</v>
+        <v>2846.7</v>
       </c>
     </row>
     <row r="222" spans="1:28" x14ac:dyDescent="0.35">
@@ -21344,7 +21351,7 @@
         <v>5814293.6820999999</v>
       </c>
       <c r="AB224">
-        <v>136.5</v>
+        <v>311.60000000000002</v>
       </c>
     </row>
     <row r="225" spans="1:28" x14ac:dyDescent="0.35">
@@ -21424,7 +21431,7 @@
         <v>5814293.6820999999</v>
       </c>
       <c r="AB225">
-        <v>136.5</v>
+        <v>311.60000000000002</v>
       </c>
     </row>
     <row r="226" spans="1:28" x14ac:dyDescent="0.35">
@@ -21504,7 +21511,7 @@
         <v>5814379.5389</v>
       </c>
       <c r="AB226">
-        <v>9.1999999999999993</v>
+        <v>61</v>
       </c>
     </row>
     <row r="227" spans="1:28" x14ac:dyDescent="0.35">
@@ -21584,7 +21591,7 @@
         <v>5814379.5389</v>
       </c>
       <c r="AB227">
-        <v>9.1999999999999993</v>
+        <v>61</v>
       </c>
     </row>
     <row r="228" spans="1:28" x14ac:dyDescent="0.35">
@@ -21664,7 +21671,7 @@
         <v>5814442.3754000003</v>
       </c>
       <c r="AB228">
-        <v>147.4</v>
+        <v>768.8</v>
       </c>
     </row>
     <row r="229" spans="1:28" x14ac:dyDescent="0.35">
@@ -21744,7 +21751,7 @@
         <v>5814560.5130000003</v>
       </c>
       <c r="AB229">
-        <v>29.2</v>
+        <v>68.599999999999994</v>
       </c>
     </row>
     <row r="230" spans="1:28" x14ac:dyDescent="0.35">
@@ -21824,7 +21831,7 @@
         <v>5814578.0299000004</v>
       </c>
       <c r="AB230">
-        <v>80.5</v>
+        <v>151</v>
       </c>
     </row>
     <row r="231" spans="1:28" x14ac:dyDescent="0.35">
@@ -21904,7 +21911,7 @@
         <v>5814623.0122999996</v>
       </c>
       <c r="AB231">
-        <v>29.3</v>
+        <v>52.400000000000006</v>
       </c>
     </row>
     <row r="232" spans="1:28" x14ac:dyDescent="0.35">
@@ -22144,7 +22151,7 @@
         <v>5814634.5289000003</v>
       </c>
       <c r="AB234">
-        <v>70.599999999999994</v>
+        <v>168.1</v>
       </c>
     </row>
     <row r="235" spans="1:28" x14ac:dyDescent="0.35">
@@ -22224,7 +22231,7 @@
         <v>5814676.9906000001</v>
       </c>
       <c r="AB235">
-        <v>168.7</v>
+        <v>263.39999999999998</v>
       </c>
     </row>
     <row r="236" spans="1:28" x14ac:dyDescent="0.35">
@@ -22304,7 +22311,7 @@
         <v>5814678.4879999999</v>
       </c>
       <c r="AB236">
-        <v>26.7</v>
+        <v>77.5</v>
       </c>
     </row>
     <row r="237" spans="1:28" x14ac:dyDescent="0.35">
@@ -22384,7 +22391,7 @@
         <v>5814678.4879999999</v>
       </c>
       <c r="AB237">
-        <v>26.7</v>
+        <v>77.5</v>
       </c>
     </row>
     <row r="238" spans="1:28" x14ac:dyDescent="0.35">
@@ -22464,7 +22471,7 @@
         <v>5814728.0266000004</v>
       </c>
       <c r="AB238">
-        <v>260.3</v>
+        <v>280.40000000000003</v>
       </c>
     </row>
     <row r="239" spans="1:28" x14ac:dyDescent="0.35">
@@ -22704,7 +22711,7 @@
         <v>5814877.9985999996</v>
       </c>
       <c r="AB241">
-        <v>25.9</v>
+        <v>152.5</v>
       </c>
     </row>
     <row r="242" spans="1:28" x14ac:dyDescent="0.35">
@@ -22784,7 +22791,7 @@
         <v>5814893.4720999999</v>
       </c>
       <c r="AB242">
-        <v>2.2000000000000002</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="243" spans="1:28" x14ac:dyDescent="0.35">
@@ -22864,7 +22871,7 @@
         <v>5815042.9956999999</v>
       </c>
       <c r="AB243">
-        <v>23.6</v>
+        <v>28.1</v>
       </c>
     </row>
     <row r="244" spans="1:28" x14ac:dyDescent="0.35">
@@ -22944,7 +22951,7 @@
         <v>5815154.5197999999</v>
       </c>
       <c r="AB244">
-        <v>7.9</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="245" spans="1:28" x14ac:dyDescent="0.35">
@@ -23344,7 +23351,7 @@
         <v>5815207.1891000001</v>
       </c>
       <c r="AB249">
-        <v>61.6</v>
+        <v>193.8</v>
       </c>
     </row>
     <row r="250" spans="1:28" x14ac:dyDescent="0.35">
@@ -23664,7 +23671,7 @@
         <v>5815223.5257999999</v>
       </c>
       <c r="AB253">
-        <v>11</v>
+        <v>53.2</v>
       </c>
     </row>
     <row r="254" spans="1:28" x14ac:dyDescent="0.35">
@@ -24224,7 +24231,7 @@
         <v>5815308.4778000005</v>
       </c>
       <c r="AB260">
-        <v>25.2</v>
+        <v>65.8</v>
       </c>
     </row>
     <row r="261" spans="1:28" x14ac:dyDescent="0.35">
@@ -24304,7 +24311,7 @@
         <v>5815309.0073999995</v>
       </c>
       <c r="AB261">
-        <v>0.3</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="262" spans="1:28" x14ac:dyDescent="0.35">
@@ -24624,7 +24631,7 @@
         <v>5815402.6692000004</v>
       </c>
       <c r="AB265">
-        <v>39</v>
+        <v>85</v>
       </c>
     </row>
     <row r="266" spans="1:28" x14ac:dyDescent="0.35">
@@ -24704,7 +24711,7 @@
         <v>5815402.6692000004</v>
       </c>
       <c r="AB266">
-        <v>39</v>
+        <v>85</v>
       </c>
     </row>
     <row r="267" spans="1:28" x14ac:dyDescent="0.35">
@@ -24784,7 +24791,7 @@
         <v>5815402.6692000004</v>
       </c>
       <c r="AB267">
-        <v>39</v>
+        <v>85</v>
       </c>
     </row>
     <row r="268" spans="1:28" x14ac:dyDescent="0.35">
@@ -24864,7 +24871,7 @@
         <v>5815404.9949000003</v>
       </c>
       <c r="AB268">
-        <v>21.2</v>
+        <v>27</v>
       </c>
     </row>
     <row r="269" spans="1:28" x14ac:dyDescent="0.35">
@@ -24944,7 +24951,7 @@
         <v>5815409.5001999997</v>
       </c>
       <c r="AB269">
-        <v>7.5</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="270" spans="1:28" x14ac:dyDescent="0.35">
@@ -25024,7 +25031,7 @@
         <v>5815409.5001999997</v>
       </c>
       <c r="AB270">
-        <v>7.5</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="271" spans="1:28" x14ac:dyDescent="0.35">
@@ -25264,7 +25271,7 @@
         <v>5815526.534</v>
       </c>
       <c r="AB273">
-        <v>12.9</v>
+        <v>21.9</v>
       </c>
     </row>
     <row r="274" spans="1:28" x14ac:dyDescent="0.35">
@@ -25344,7 +25351,7 @@
         <v>5815526.534</v>
       </c>
       <c r="AB274">
-        <v>12.9</v>
+        <v>21.9</v>
       </c>
     </row>
     <row r="275" spans="1:28" x14ac:dyDescent="0.35">
@@ -25744,7 +25751,7 @@
         <v>5815748.3076999998</v>
       </c>
       <c r="AB279">
-        <v>3.7</v>
+        <v>18.399999999999999</v>
       </c>
     </row>
     <row r="280" spans="1:28" x14ac:dyDescent="0.35">
@@ -25824,7 +25831,7 @@
         <v>5815748.3076999998</v>
       </c>
       <c r="AB280">
-        <v>3.7</v>
+        <v>18.399999999999999</v>
       </c>
     </row>
     <row r="281" spans="1:28" x14ac:dyDescent="0.35">
@@ -25904,7 +25911,7 @@
         <v>5815805.5014000004</v>
       </c>
       <c r="AB281">
-        <v>13.6</v>
+        <v>16.899999999999999</v>
       </c>
     </row>
     <row r="282" spans="1:28" x14ac:dyDescent="0.35">
@@ -26144,7 +26151,7 @@
         <v>5815986.3245999999</v>
       </c>
       <c r="AB284">
-        <v>1.4</v>
+        <v>78.699999999999989</v>
       </c>
     </row>
     <row r="285" spans="1:28" x14ac:dyDescent="0.35">
@@ -26224,7 +26231,7 @@
         <v>5815986.3245999999</v>
       </c>
       <c r="AB285">
-        <v>1.4</v>
+        <v>78.699999999999989</v>
       </c>
     </row>
     <row r="286" spans="1:28" x14ac:dyDescent="0.35">
@@ -26304,7 +26311,7 @@
         <v>5816020.9733999996</v>
       </c>
       <c r="AB286">
-        <v>103</v>
+        <v>228.10000000000002</v>
       </c>
     </row>
     <row r="287" spans="1:28" x14ac:dyDescent="0.35">
@@ -26384,7 +26391,7 @@
         <v>5816020.9733999996</v>
       </c>
       <c r="AB287">
-        <v>103</v>
+        <v>228.10000000000002</v>
       </c>
     </row>
     <row r="288" spans="1:28" x14ac:dyDescent="0.35">
@@ -26464,7 +26471,7 @@
         <v>5816054.5099999998</v>
       </c>
       <c r="AB288">
-        <v>7.4</v>
+        <v>9.2000000000000011</v>
       </c>
     </row>
     <row r="289" spans="1:28" x14ac:dyDescent="0.35">
@@ -26544,7 +26551,7 @@
         <v>5816057.0036000004</v>
       </c>
       <c r="AB289">
-        <v>0.2</v>
+        <v>7.1000000000000005</v>
       </c>
     </row>
     <row r="290" spans="1:28" x14ac:dyDescent="0.35">
@@ -26704,7 +26711,7 @@
         <v>5816308.5092000002</v>
       </c>
       <c r="AB291">
-        <v>11.7</v>
+        <v>15.299999999999999</v>
       </c>
     </row>
     <row r="292" spans="1:28" x14ac:dyDescent="0.35">
@@ -26784,7 +26791,7 @@
         <v>5816360.0089999996</v>
       </c>
       <c r="AB292">
-        <v>0.4</v>
+        <v>8.7000000000000011</v>
       </c>
     </row>
     <row r="293" spans="1:28" x14ac:dyDescent="0.35">
@@ -26864,7 +26871,7 @@
         <v>5816360.0089999996</v>
       </c>
       <c r="AB293">
-        <v>0.4</v>
+        <v>8.7000000000000011</v>
       </c>
     </row>
     <row r="294" spans="1:28" x14ac:dyDescent="0.35">
@@ -27024,7 +27031,7 @@
         <v>5816546.0193999996</v>
       </c>
       <c r="AB295">
-        <v>1.5</v>
+        <v>21.4</v>
       </c>
     </row>
     <row r="296" spans="1:28" x14ac:dyDescent="0.35">
@@ -27104,7 +27111,7 @@
         <v>5816569.9813999999</v>
       </c>
       <c r="AB296">
-        <v>1.9</v>
+        <v>26.9</v>
       </c>
     </row>
     <row r="297" spans="1:28" x14ac:dyDescent="0.35">
@@ -27184,7 +27191,7 @@
         <v>5816569.9813999999</v>
       </c>
       <c r="AB297">
-        <v>1.9</v>
+        <v>26.9</v>
       </c>
     </row>
     <row r="298" spans="1:28" x14ac:dyDescent="0.35">
@@ -27264,7 +27271,7 @@
         <v>5816580.3015999999</v>
       </c>
       <c r="AB298">
-        <v>19.7</v>
+        <v>160.30000000000001</v>
       </c>
     </row>
     <row r="299" spans="1:28" x14ac:dyDescent="0.35">
@@ -27344,7 +27351,7 @@
         <v>5816580.3015999999</v>
       </c>
       <c r="AB299">
-        <v>19.7</v>
+        <v>160.30000000000001</v>
       </c>
     </row>
     <row r="300" spans="1:28" x14ac:dyDescent="0.35">
@@ -27424,7 +27431,7 @@
         <v>5816681.4603000004</v>
       </c>
       <c r="AB300">
-        <v>19.7</v>
+        <v>36.599999999999994</v>
       </c>
     </row>
     <row r="301" spans="1:28" x14ac:dyDescent="0.35">
@@ -27504,7 +27511,7 @@
         <v>5816770.0073999995</v>
       </c>
       <c r="AB301">
-        <v>14.2</v>
+        <v>41.5</v>
       </c>
     </row>
     <row r="302" spans="1:28" x14ac:dyDescent="0.35">
@@ -27584,7 +27591,7 @@
         <v>5816846.9844000004</v>
       </c>
       <c r="AB302">
-        <v>17.899999999999999</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="303" spans="1:28" x14ac:dyDescent="0.35">
@@ -27664,7 +27671,7 @@
         <v>5816846.9844000004</v>
       </c>
       <c r="AB303">
-        <v>17.899999999999999</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="304" spans="1:28" x14ac:dyDescent="0.35">
@@ -27824,7 +27831,7 @@
         <v>5816892.9636000004</v>
       </c>
       <c r="AB305">
-        <v>38.700000000000003</v>
+        <v>57.2</v>
       </c>
     </row>
     <row r="306" spans="1:28" x14ac:dyDescent="0.35">
@@ -28064,7 +28071,7 @@
         <v>5816996.9704</v>
       </c>
       <c r="AB308">
-        <v>33.5</v>
+        <v>35.700000000000003</v>
       </c>
     </row>
     <row r="309" spans="1:28" x14ac:dyDescent="0.35">
@@ -28144,7 +28151,7 @@
         <v>5817001.9884000001</v>
       </c>
       <c r="AB309">
-        <v>15.1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="310" spans="1:28" x14ac:dyDescent="0.35">
@@ -28224,7 +28231,7 @@
         <v>5817025.4594999999</v>
       </c>
       <c r="AB310">
-        <v>44</v>
+        <v>45.4</v>
       </c>
     </row>
     <row r="311" spans="1:28" x14ac:dyDescent="0.35">
@@ -28384,7 +28391,7 @@
         <v>5817069.9981000004</v>
       </c>
       <c r="AB312">
-        <v>0.2</v>
+        <v>2.3000000000000003</v>
       </c>
     </row>
     <row r="313" spans="1:28" x14ac:dyDescent="0.35">
@@ -28464,7 +28471,7 @@
         <v>5817069.9981000004</v>
       </c>
       <c r="AB313">
-        <v>0.2</v>
+        <v>2.3000000000000003</v>
       </c>
     </row>
     <row r="314" spans="1:28" x14ac:dyDescent="0.35">
@@ -28544,7 +28551,7 @@
         <v>5817069.9981000004</v>
       </c>
       <c r="AB314">
-        <v>0.2</v>
+        <v>2.3000000000000003</v>
       </c>
     </row>
     <row r="315" spans="1:28" x14ac:dyDescent="0.35">
@@ -28624,7 +28631,7 @@
         <v>5817080.4800000004</v>
       </c>
       <c r="AB315">
-        <v>17.600000000000001</v>
+        <v>22.400000000000002</v>
       </c>
     </row>
     <row r="316" spans="1:28" x14ac:dyDescent="0.35">
@@ -28704,7 +28711,7 @@
         <v>5817094.9879000001</v>
       </c>
       <c r="AB316">
-        <v>8</v>
+        <v>23.6</v>
       </c>
     </row>
     <row r="317" spans="1:28" x14ac:dyDescent="0.35">
@@ -28784,7 +28791,7 @@
         <v>5817383.9878000002</v>
       </c>
       <c r="AB317">
-        <v>1.4</v>
+        <v>9.6</v>
       </c>
     </row>
     <row r="318" spans="1:28" x14ac:dyDescent="0.35">
@@ -28944,7 +28951,7 @@
         <v>5817389.0109999999</v>
       </c>
       <c r="AB319">
-        <v>0.4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="320" spans="1:28" x14ac:dyDescent="0.35">
@@ -29024,7 +29031,7 @@
         <v>5817389.0109999999</v>
       </c>
       <c r="AB320">
-        <v>0.4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="321" spans="1:28" x14ac:dyDescent="0.35">
@@ -29104,7 +29111,7 @@
         <v>5817397.0362999998</v>
       </c>
       <c r="AB321">
-        <v>37.799999999999997</v>
+        <v>45</v>
       </c>
     </row>
     <row r="322" spans="1:28" x14ac:dyDescent="0.35">
@@ -29184,7 +29191,7 @@
         <v>5817470.5261000004</v>
       </c>
       <c r="AB322">
-        <v>46.9</v>
+        <v>64.7</v>
       </c>
     </row>
     <row r="323" spans="1:28" x14ac:dyDescent="0.35">
@@ -29264,7 +29271,7 @@
         <v>5817571.0056999996</v>
       </c>
       <c r="AB323">
-        <v>58.5</v>
+        <v>138.6</v>
       </c>
     </row>
     <row r="324" spans="1:28" x14ac:dyDescent="0.35">
@@ -29424,7 +29431,7 @@
         <v>5817607.9929</v>
       </c>
       <c r="AB325">
-        <v>9.5</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="326" spans="1:28" x14ac:dyDescent="0.35">
@@ -29504,7 +29511,7 @@
         <v>5817608.4851000002</v>
       </c>
       <c r="AB326">
-        <v>0.7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="327" spans="1:28" x14ac:dyDescent="0.35">
@@ -29584,7 +29591,7 @@
         <v>5817608.4851000002</v>
       </c>
       <c r="AB327">
-        <v>0.7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="328" spans="1:28" x14ac:dyDescent="0.35">
@@ -29664,7 +29671,7 @@
         <v>5817652.0048000002</v>
       </c>
       <c r="AB328">
-        <v>0.7</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="329" spans="1:28" x14ac:dyDescent="0.35">
@@ -29744,7 +29751,7 @@
         <v>5817662.9720000001</v>
       </c>
       <c r="AB329">
-        <v>6.2</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="330" spans="1:28" x14ac:dyDescent="0.35">
@@ -29824,7 +29831,7 @@
         <v>5817662.9720000001</v>
       </c>
       <c r="AB330">
-        <v>6.2</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="331" spans="1:28" x14ac:dyDescent="0.35">
@@ -29904,7 +29911,7 @@
         <v>5817669.9540999997</v>
       </c>
       <c r="AB331">
-        <v>0.8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="332" spans="1:28" x14ac:dyDescent="0.35">
@@ -29984,7 +29991,7 @@
         <v>5817697.0286999997</v>
       </c>
       <c r="AB332">
-        <v>25.7</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="333" spans="1:28" x14ac:dyDescent="0.35">
@@ -30064,7 +30071,7 @@
         <v>5817698.0125000002</v>
       </c>
       <c r="AB333">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="334" spans="1:28" x14ac:dyDescent="0.35">
@@ -30144,7 +30151,7 @@
         <v>5817702.4971000003</v>
       </c>
       <c r="AB334">
-        <v>7</v>
+        <v>35.200000000000003</v>
       </c>
     </row>
     <row r="335" spans="1:28" x14ac:dyDescent="0.35">
@@ -30304,7 +30311,7 @@
         <v>5817730.5336999996</v>
       </c>
       <c r="AB336">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="337" spans="1:28" x14ac:dyDescent="0.35">
@@ -30384,7 +30391,7 @@
         <v>5817752.4970000004</v>
       </c>
       <c r="AB337">
-        <v>0.6</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="338" spans="1:28" x14ac:dyDescent="0.35">
@@ -30464,7 +30471,7 @@
         <v>5817752.4970000004</v>
       </c>
       <c r="AB338">
-        <v>0.6</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="339" spans="1:28" x14ac:dyDescent="0.35">
@@ -30544,7 +30551,7 @@
         <v>5817760.4694999997</v>
       </c>
       <c r="AB339">
-        <v>7.1</v>
+        <v>10.399999999999999</v>
       </c>
     </row>
     <row r="340" spans="1:28" x14ac:dyDescent="0.35">
@@ -30624,7 +30631,7 @@
         <v>5817760.4694999997</v>
       </c>
       <c r="AB340">
-        <v>7.1</v>
+        <v>10.399999999999999</v>
       </c>
     </row>
     <row r="341" spans="1:28" x14ac:dyDescent="0.35">
@@ -30704,7 +30711,7 @@
         <v>5817894.9802999999</v>
       </c>
       <c r="AB341">
-        <v>85</v>
+        <v>101.3</v>
       </c>
     </row>
     <row r="342" spans="1:28" x14ac:dyDescent="0.35">
@@ -30784,7 +30791,7 @@
         <v>5817964.1642000005</v>
       </c>
       <c r="AB342">
-        <v>9.6</v>
+        <v>41.400000000000006</v>
       </c>
     </row>
     <row r="343" spans="1:28" x14ac:dyDescent="0.35">
@@ -31104,7 +31111,7 @@
         <v>5818076.4903999995</v>
       </c>
       <c r="AB346">
-        <v>37.799999999999997</v>
+        <v>69</v>
       </c>
     </row>
     <row r="347" spans="1:28" x14ac:dyDescent="0.35">
@@ -31184,7 +31191,7 @@
         <v>5818076.7812999999</v>
       </c>
       <c r="AB347">
-        <v>62.6</v>
+        <v>826.5</v>
       </c>
     </row>
     <row r="348" spans="1:28" x14ac:dyDescent="0.35">
@@ -31264,7 +31271,7 @@
         <v>5818082.0214999998</v>
       </c>
       <c r="AB348">
-        <v>68.8</v>
+        <v>123.3</v>
       </c>
     </row>
     <row r="349" spans="1:28" x14ac:dyDescent="0.35">
@@ -31344,7 +31351,7 @@
         <v>5818149.4819</v>
       </c>
       <c r="AB349">
-        <v>31.9</v>
+        <v>90.199999999999989</v>
       </c>
     </row>
     <row r="350" spans="1:28" x14ac:dyDescent="0.35">
@@ -31424,7 +31431,7 @@
         <v>5818244.4900000002</v>
       </c>
       <c r="AB350">
-        <v>12</v>
+        <v>91.8</v>
       </c>
     </row>
     <row r="351" spans="1:28" x14ac:dyDescent="0.35">
@@ -31504,7 +31511,7 @@
         <v>5818282.5157000003</v>
       </c>
       <c r="AB351">
-        <v>21.8</v>
+        <v>76.7</v>
       </c>
     </row>
     <row r="352" spans="1:28" x14ac:dyDescent="0.35">
@@ -31584,7 +31591,7 @@
         <v>5818310.0146000003</v>
       </c>
       <c r="AB352">
-        <v>0.4</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="353" spans="1:28" x14ac:dyDescent="0.35">
@@ -31664,7 +31671,7 @@
         <v>5818493.9700999996</v>
       </c>
       <c r="AB353">
-        <v>0.8</v>
+        <v>20.2</v>
       </c>
     </row>
     <row r="354" spans="1:28" x14ac:dyDescent="0.35">
@@ -31744,7 +31751,7 @@
         <v>5818588.9979999997</v>
       </c>
       <c r="AB354">
-        <v>0.1</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="355" spans="1:28" x14ac:dyDescent="0.35">
@@ -31824,7 +31831,7 @@
         <v>5818656.0122999996</v>
       </c>
       <c r="AB355">
-        <v>24.4</v>
+        <v>25.799999999999997</v>
       </c>
     </row>
     <row r="356" spans="1:28" x14ac:dyDescent="0.35">
@@ -31904,7 +31911,7 @@
         <v>5818656.0122999996</v>
       </c>
       <c r="AB356">
-        <v>24.4</v>
+        <v>25.799999999999997</v>
       </c>
     </row>
     <row r="357" spans="1:28" x14ac:dyDescent="0.35">
@@ -31984,7 +31991,7 @@
         <v>5818747.4845000003</v>
       </c>
       <c r="AB357">
-        <v>3</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="358" spans="1:28" x14ac:dyDescent="0.35">
@@ -32064,7 +32071,7 @@
         <v>5818766.0245000003</v>
       </c>
       <c r="AB358">
-        <v>58.7</v>
+        <v>68.3</v>
       </c>
     </row>
     <row r="359" spans="1:28" x14ac:dyDescent="0.35">
@@ -32224,7 +32231,7 @@
         <v>5818970.9738999996</v>
       </c>
       <c r="AB360">
-        <v>8.8000000000000007</v>
+        <v>29.6</v>
       </c>
     </row>
     <row r="361" spans="1:28" x14ac:dyDescent="0.35">
@@ -32304,7 +32311,7 @@
         <v>5818975.4885</v>
       </c>
       <c r="AB361">
-        <v>82.6</v>
+        <v>116.89999999999999</v>
       </c>
     </row>
     <row r="362" spans="1:28" x14ac:dyDescent="0.35">
@@ -32384,7 +32391,7 @@
         <v>5818975.4885</v>
       </c>
       <c r="AB362">
-        <v>82.6</v>
+        <v>116.89999999999999</v>
       </c>
     </row>
     <row r="363" spans="1:28" x14ac:dyDescent="0.35">
@@ -32464,7 +32471,7 @@
         <v>5819052.4588000001</v>
       </c>
       <c r="AB363">
-        <v>27</v>
+        <v>42.6</v>
       </c>
     </row>
     <row r="364" spans="1:28" x14ac:dyDescent="0.35">
@@ -32544,7 +32551,7 @@
         <v>5819052.4588000001</v>
       </c>
       <c r="AB364">
-        <v>27</v>
+        <v>42.6</v>
       </c>
     </row>
     <row r="365" spans="1:28" x14ac:dyDescent="0.35">
@@ -32703,8 +32710,8 @@
       <c r="AA366">
         <v>5819206.3502000002</v>
       </c>
-      <c r="AB366" t="e">
-        <v>#N/A</v>
+      <c r="AB366">
+        <v>348.5</v>
       </c>
     </row>
     <row r="367" spans="1:28" x14ac:dyDescent="0.35">
@@ -32784,7 +32791,7 @@
         <v>5819222.3520999998</v>
       </c>
       <c r="AB367">
-        <v>40</v>
+        <v>55.699999999999996</v>
       </c>
     </row>
     <row r="368" spans="1:28" x14ac:dyDescent="0.35">
@@ -32864,7 +32871,7 @@
         <v>5819247.4918999998</v>
       </c>
       <c r="AB368">
-        <v>11.8</v>
+        <v>45.900000000000006</v>
       </c>
     </row>
     <row r="369" spans="1:28" x14ac:dyDescent="0.35">
@@ -33024,7 +33031,7 @@
         <v>5819296.5416000001</v>
       </c>
       <c r="AB370">
-        <v>7.8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="371" spans="1:28" x14ac:dyDescent="0.35">
@@ -33104,7 +33111,7 @@
         <v>5819329.4996999996</v>
       </c>
       <c r="AB371">
-        <v>2.4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="372" spans="1:28" x14ac:dyDescent="0.35">
@@ -33184,7 +33191,7 @@
         <v>5819374.0104999999</v>
       </c>
       <c r="AB372">
-        <v>55.2</v>
+        <v>117.6</v>
       </c>
     </row>
     <row r="373" spans="1:28" x14ac:dyDescent="0.35">
@@ -33264,7 +33271,7 @@
         <v>5819374.0104999999</v>
       </c>
       <c r="AB373">
-        <v>55.2</v>
+        <v>117.6</v>
       </c>
     </row>
     <row r="374" spans="1:28" x14ac:dyDescent="0.35">
@@ -33344,7 +33351,7 @@
         <v>5819400.9863999998</v>
       </c>
       <c r="AB374">
-        <v>20.6</v>
+        <v>39</v>
       </c>
     </row>
     <row r="375" spans="1:28" x14ac:dyDescent="0.35">
@@ -33504,7 +33511,7 @@
         <v>5819577.0215999996</v>
       </c>
       <c r="AB376">
-        <v>16.5</v>
+        <v>50.1</v>
       </c>
     </row>
     <row r="377" spans="1:28" x14ac:dyDescent="0.35">
@@ -33584,7 +33591,7 @@
         <v>5819781.4539000001</v>
       </c>
       <c r="AB377">
-        <v>17.399999999999999</v>
+        <v>51.4</v>
       </c>
     </row>
     <row r="378" spans="1:28" x14ac:dyDescent="0.35">
@@ -33664,7 +33671,7 @@
         <v>5819781.4539000001</v>
       </c>
       <c r="AB378">
-        <v>17.399999999999999</v>
+        <v>51.4</v>
       </c>
     </row>
     <row r="379" spans="1:28" x14ac:dyDescent="0.35">
@@ -33904,7 +33911,7 @@
         <v>5819822.4656999996</v>
       </c>
       <c r="AB381">
-        <v>38.700000000000003</v>
+        <v>84.9</v>
       </c>
     </row>
     <row r="382" spans="1:28" x14ac:dyDescent="0.35">
@@ -34224,7 +34231,7 @@
         <v>5820122.9768000003</v>
       </c>
       <c r="AB385">
-        <v>10.7</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="386" spans="1:28" x14ac:dyDescent="0.35">
@@ -34304,7 +34311,7 @@
         <v>5820166.0273000002</v>
       </c>
       <c r="AB386">
-        <v>2.6</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="387" spans="1:28" x14ac:dyDescent="0.35">
@@ -34384,7 +34391,7 @@
         <v>5820180.5001999997</v>
       </c>
       <c r="AB387">
-        <v>43.7</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="388" spans="1:28" x14ac:dyDescent="0.35">
@@ -34464,7 +34471,7 @@
         <v>5820180.5001999997</v>
       </c>
       <c r="AB388">
-        <v>43.7</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="389" spans="1:28" x14ac:dyDescent="0.35">
@@ -34544,7 +34551,7 @@
         <v>5820314.4952999996</v>
       </c>
       <c r="AB389">
-        <v>4.0999999999999996</v>
+        <v>8.6</v>
       </c>
     </row>
     <row r="390" spans="1:28" x14ac:dyDescent="0.35">
@@ -34624,7 +34631,7 @@
         <v>5820394.4939000001</v>
       </c>
       <c r="AB390">
-        <v>0.3</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="391" spans="1:28" x14ac:dyDescent="0.35">
@@ -34704,7 +34711,7 @@
         <v>5820529.9990999997</v>
       </c>
       <c r="AB391">
-        <v>24.6</v>
+        <v>42.5</v>
       </c>
     </row>
     <row r="392" spans="1:28" x14ac:dyDescent="0.35">
@@ -34784,7 +34791,7 @@
         <v>5820552.5165999997</v>
       </c>
       <c r="AB392">
-        <v>10.199999999999999</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="393" spans="1:28" x14ac:dyDescent="0.35">
@@ -34864,7 +34871,7 @@
         <v>5820554.4740000004</v>
       </c>
       <c r="AB393">
-        <v>41.8</v>
+        <v>63.9</v>
       </c>
     </row>
     <row r="394" spans="1:28" x14ac:dyDescent="0.35">
@@ -34944,7 +34951,7 @@
         <v>5820554.4740000004</v>
       </c>
       <c r="AB394">
-        <v>41.8</v>
+        <v>63.9</v>
       </c>
     </row>
     <row r="395" spans="1:28" x14ac:dyDescent="0.35">
@@ -35024,7 +35031,7 @@
         <v>5820708.0176999997</v>
       </c>
       <c r="AB395">
-        <v>59.7</v>
+        <v>110.4</v>
       </c>
     </row>
     <row r="396" spans="1:28" x14ac:dyDescent="0.35">
@@ -35104,7 +35111,7 @@
         <v>5820708.0176999997</v>
       </c>
       <c r="AB396">
-        <v>59.7</v>
+        <v>110.4</v>
       </c>
     </row>
     <row r="397" spans="1:28" x14ac:dyDescent="0.35">
@@ -35184,7 +35191,7 @@
         <v>5820788.9839000003</v>
       </c>
       <c r="AB397">
-        <v>14.6</v>
+        <v>30.700000000000003</v>
       </c>
     </row>
     <row r="398" spans="1:28" x14ac:dyDescent="0.35">
@@ -35264,7 +35271,7 @@
         <v>5820828.4906000001</v>
       </c>
       <c r="AB398">
-        <v>54.8</v>
+        <v>149.19999999999999</v>
       </c>
     </row>
     <row r="399" spans="1:28" x14ac:dyDescent="0.35">
@@ -35344,7 +35351,7 @@
         <v>5820957.0077999998</v>
       </c>
       <c r="AB399">
-        <v>175</v>
+        <v>720.3</v>
       </c>
     </row>
     <row r="400" spans="1:28" x14ac:dyDescent="0.35">
@@ -35664,7 +35671,7 @@
         <v>5821165.3272000002</v>
       </c>
       <c r="AB403">
-        <v>56.9</v>
+        <v>94.9</v>
       </c>
     </row>
     <row r="404" spans="1:28" x14ac:dyDescent="0.35">
@@ -35744,7 +35751,7 @@
         <v>5821167.9802999999</v>
       </c>
       <c r="AB404">
-        <v>3.1</v>
+        <v>48.3</v>
       </c>
     </row>
     <row r="405" spans="1:28" x14ac:dyDescent="0.35">
@@ -35824,7 +35831,7 @@
         <v>5821307.0325999996</v>
       </c>
       <c r="AB405">
-        <v>116.1</v>
+        <v>179.8</v>
       </c>
     </row>
     <row r="406" spans="1:28" x14ac:dyDescent="0.35">
@@ -35904,7 +35911,7 @@
         <v>5821400.6925999997</v>
       </c>
       <c r="AB406">
-        <v>0.9</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="407" spans="1:28" x14ac:dyDescent="0.35">
@@ -35984,7 +35991,7 @@
         <v>5821432.2300000004</v>
       </c>
       <c r="AB407">
-        <v>89.4</v>
+        <v>137.60000000000002</v>
       </c>
     </row>
     <row r="408" spans="1:28" x14ac:dyDescent="0.35">
@@ -36064,7 +36071,7 @@
         <v>5821432.2300000004</v>
       </c>
       <c r="AB408">
-        <v>89.4</v>
+        <v>137.60000000000002</v>
       </c>
     </row>
     <row r="409" spans="1:28" x14ac:dyDescent="0.35">
@@ -36144,7 +36151,7 @@
         <v>5821502.0329</v>
       </c>
       <c r="AB409">
-        <v>0.7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="410" spans="1:28" x14ac:dyDescent="0.35">
@@ -36224,7 +36231,7 @@
         <v>5821709.6584999999</v>
       </c>
       <c r="AB410">
-        <v>0.3</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="411" spans="1:28" x14ac:dyDescent="0.35">
@@ -36304,7 +36311,7 @@
         <v>5821709.6584999999</v>
       </c>
       <c r="AB411">
-        <v>0.3</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="412" spans="1:28" x14ac:dyDescent="0.35">
@@ -36544,7 +36551,7 @@
         <v>5822100.4515000004</v>
       </c>
       <c r="AB414">
-        <v>1.7</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="415" spans="1:28" x14ac:dyDescent="0.35">
@@ -36624,7 +36631,7 @@
         <v>5822100.4515000004</v>
       </c>
       <c r="AB415">
-        <v>1.7</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="416" spans="1:28" x14ac:dyDescent="0.35">
@@ -36704,7 +36711,7 @@
         <v>5822100.4515000004</v>
       </c>
       <c r="AB416">
-        <v>1.7</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="417" spans="1:28" x14ac:dyDescent="0.35">
@@ -36784,7 +36791,7 @@
         <v>5822100.4515000004</v>
       </c>
       <c r="AB417">
-        <v>1.7</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="418" spans="1:28" x14ac:dyDescent="0.35">
@@ -36944,7 +36951,7 @@
         <v>5822187.2344000004</v>
       </c>
       <c r="AB419">
-        <v>2.4</v>
+        <v>22.400000000000002</v>
       </c>
     </row>
     <row r="420" spans="1:28" x14ac:dyDescent="0.35">
@@ -37184,7 +37191,7 @@
         <v>5822357.6206999999</v>
       </c>
       <c r="AB422">
-        <v>4.5999999999999996</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="423" spans="1:28" x14ac:dyDescent="0.35">
@@ -37264,7 +37271,7 @@
         <v>5822394.5163000003</v>
       </c>
       <c r="AB423">
-        <v>2.4</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="424" spans="1:28" x14ac:dyDescent="0.35">
@@ -37424,7 +37431,7 @@
         <v>5822569.9970000004</v>
       </c>
       <c r="AB425">
-        <v>3.3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="426" spans="1:28" x14ac:dyDescent="0.35">
@@ -37504,7 +37511,7 @@
         <v>5822569.9970000004</v>
       </c>
       <c r="AB426">
-        <v>3.3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="427" spans="1:28" x14ac:dyDescent="0.35">
@@ -37584,7 +37591,7 @@
         <v>5822615.0244000005</v>
       </c>
       <c r="AB427">
-        <v>3.2</v>
+        <v>3.4000000000000004</v>
       </c>
     </row>
     <row r="428" spans="1:28" x14ac:dyDescent="0.35">
@@ -37744,7 +37751,7 @@
         <v>5822728.4720000001</v>
       </c>
       <c r="AB429">
-        <v>1.6</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="430" spans="1:28" x14ac:dyDescent="0.35">
@@ -38144,7 +38151,7 @@
         <v>5822945.4988000002</v>
       </c>
       <c r="AB434">
-        <v>2.8</v>
+        <v>15.3</v>
       </c>
     </row>
     <row r="435" spans="1:28" x14ac:dyDescent="0.35">
@@ -38224,7 +38231,7 @@
         <v>5822945.4988000002</v>
       </c>
       <c r="AB435">
-        <v>2.8</v>
+        <v>15.3</v>
       </c>
     </row>
     <row r="436" spans="1:28" x14ac:dyDescent="0.35">
@@ -38304,7 +38311,7 @@
         <v>5822997.4899000004</v>
       </c>
       <c r="AB436">
-        <v>1.6</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="437" spans="1:28" x14ac:dyDescent="0.35">
@@ -38384,7 +38391,7 @@
         <v>5822997.4899000004</v>
       </c>
       <c r="AB437">
-        <v>1.6</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="438" spans="1:28" x14ac:dyDescent="0.35">
@@ -38464,7 +38471,7 @@
         <v>5823170.4538000003</v>
       </c>
       <c r="AB438">
-        <v>1.2</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="439" spans="1:28" x14ac:dyDescent="0.35">
@@ -38544,7 +38551,7 @@
         <v>5823417.9737</v>
       </c>
       <c r="AB439">
-        <v>1.4</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="440" spans="1:28" x14ac:dyDescent="0.35">
@@ -38624,7 +38631,7 @@
         <v>5823593.4918999998</v>
       </c>
       <c r="AB440">
-        <v>1.7</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="441" spans="1:28" x14ac:dyDescent="0.35">
@@ -38704,7 +38711,7 @@
         <v>5823777.6157</v>
       </c>
       <c r="AB441">
-        <v>8.4</v>
+        <v>100.7</v>
       </c>
     </row>
     <row r="442" spans="1:28" x14ac:dyDescent="0.35">
@@ -38864,7 +38871,7 @@
         <v>5823842.0047000004</v>
       </c>
       <c r="AB443">
-        <v>50.4</v>
+        <v>79.900000000000006</v>
       </c>
     </row>
     <row r="444" spans="1:28" x14ac:dyDescent="0.35">
@@ -38944,7 +38951,7 @@
         <v>5823902.2986000003</v>
       </c>
       <c r="AB444">
-        <v>43.1</v>
+        <v>372.20000000000005</v>
       </c>
     </row>
     <row r="445" spans="1:28" x14ac:dyDescent="0.35">
@@ -39024,7 +39031,7 @@
         <v>5823907.9641000004</v>
       </c>
       <c r="AB445">
-        <v>28.8</v>
+        <v>31.7</v>
       </c>
     </row>
     <row r="446" spans="1:28" x14ac:dyDescent="0.35">
@@ -39504,7 +39511,7 @@
         <v>5824787.6524999999</v>
       </c>
       <c r="AB451">
-        <v>1</v>
+        <v>11.1</v>
       </c>
     </row>
     <row r="452" spans="1:28" x14ac:dyDescent="0.35">
@@ -39584,7 +39591,7 @@
         <v>5824787.6524999999</v>
       </c>
       <c r="AB452">
-        <v>1</v>
+        <v>11.1</v>
       </c>
     </row>
     <row r="453" spans="1:28" x14ac:dyDescent="0.35">
@@ -39984,7 +39991,7 @@
         <v>5825598.9989</v>
       </c>
       <c r="AB457">
-        <v>5.3</v>
+        <v>8.1999999999999993</v>
       </c>
     </row>
     <row r="458" spans="1:28" x14ac:dyDescent="0.35">
@@ -40224,7 +40231,7 @@
         <v>5826171.4919999996</v>
       </c>
       <c r="AB460">
-        <v>17</v>
+        <v>48.5</v>
       </c>
     </row>
     <row r="461" spans="1:28" x14ac:dyDescent="0.35">
@@ -40304,7 +40311,7 @@
         <v>5826674.9866000004</v>
       </c>
       <c r="AB461">
-        <v>7.2</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="462" spans="1:28" x14ac:dyDescent="0.35">
@@ -40384,7 +40391,7 @@
         <v>5826934.4791000001</v>
       </c>
       <c r="AB462">
-        <v>14.7</v>
+        <v>23.7</v>
       </c>
     </row>
     <row r="463" spans="1:28" x14ac:dyDescent="0.35">
@@ -40464,7 +40471,7 @@
         <v>5827604.6810999997</v>
       </c>
       <c r="AB463">
-        <v>26.6</v>
+        <v>75.800000000000011</v>
       </c>
     </row>
     <row r="464" spans="1:28" x14ac:dyDescent="0.35">
@@ -40544,7 +40551,7 @@
         <v>5827604.6810999997</v>
       </c>
       <c r="AB464">
-        <v>26.6</v>
+        <v>75.800000000000011</v>
       </c>
     </row>
     <row r="465" spans="1:28" x14ac:dyDescent="0.35">
@@ -40944,10 +40951,11 @@
         <v>5828111.0318</v>
       </c>
       <c r="AB469">
-        <v>8</v>
+        <v>19.7</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AB469" xr:uid="{5A5BC7F6-FFAF-4665-A239-5061DA6AB0BC}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -40956,8 +40964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F99368-5408-425B-8BA2-0870DC639DA5}">
   <dimension ref="A1:AB192"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -41125,7 +41133,7 @@
         <v>5753409.0012999997</v>
       </c>
       <c r="AB2">
-        <v>0.7</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.35">
@@ -41445,7 +41453,7 @@
         <v>5776670.1273999996</v>
       </c>
       <c r="AB6">
-        <v>461.1</v>
+        <v>1696.8999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.35">
@@ -41525,7 +41533,7 @@
         <v>5779074.0246000001</v>
       </c>
       <c r="AB7">
-        <v>30.4</v>
+        <v>191.9</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.35">
@@ -41605,7 +41613,7 @@
         <v>5780976.6639999999</v>
       </c>
       <c r="AB8">
-        <v>5.4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.35">
@@ -41685,7 +41693,7 @@
         <v>5781701.1852000002</v>
       </c>
       <c r="AB9">
-        <v>125.7</v>
+        <v>786.8</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.35">
@@ -41925,7 +41933,7 @@
         <v>5785220.9697000002</v>
       </c>
       <c r="AB12">
-        <v>13.8</v>
+        <v>37.299999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.35">
@@ -42165,7 +42173,7 @@
         <v>5786727.0175999999</v>
       </c>
       <c r="AB15">
-        <v>24.5</v>
+        <v>257.7</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.35">
@@ -42245,7 +42253,7 @@
         <v>5787278.0049000001</v>
       </c>
       <c r="AB16">
-        <v>13.4</v>
+        <v>50.900000000000006</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.35">
@@ -42325,7 +42333,7 @@
         <v>5788268.7783000004</v>
       </c>
       <c r="AB17">
-        <v>3</v>
+        <v>103.60000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.35">
@@ -42645,7 +42653,7 @@
         <v>5789848.0009000003</v>
       </c>
       <c r="AB21">
-        <v>340.4</v>
+        <v>582.59999999999991</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.35">
@@ -42725,7 +42733,7 @@
         <v>5790803.5356000001</v>
       </c>
       <c r="AB22">
-        <v>128</v>
+        <v>450.1</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.35">
@@ -42805,7 +42813,7 @@
         <v>5791783.0089999996</v>
       </c>
       <c r="AB23">
-        <v>3.5</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.35">
@@ -42885,7 +42893,7 @@
         <v>5793202.5038999999</v>
       </c>
       <c r="AB24">
-        <v>31.8</v>
+        <v>39.700000000000003</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.35">
@@ -42965,7 +42973,7 @@
         <v>5793326.9907999998</v>
       </c>
       <c r="AB25">
-        <v>0.9</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.35">
@@ -43045,7 +43053,7 @@
         <v>5793821.6047999999</v>
       </c>
       <c r="AB26">
-        <v>1116</v>
+        <v>3684.7000000000003</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.35">
@@ -43125,7 +43133,7 @@
         <v>5794440.4830999998</v>
       </c>
       <c r="AB27">
-        <v>40.799999999999997</v>
+        <v>623.4</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.35">
@@ -43205,7 +43213,7 @@
         <v>5794516.6791000003</v>
       </c>
       <c r="AB28">
-        <v>1.5</v>
+        <v>80.099999999999994</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.35">
@@ -43605,7 +43613,7 @@
         <v>5797806.0044999998</v>
       </c>
       <c r="AB33">
-        <v>171.3</v>
+        <v>309.70000000000005</v>
       </c>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.35">
@@ -43685,7 +43693,7 @@
         <v>5798071.0471999999</v>
       </c>
       <c r="AB34">
-        <v>122.4</v>
+        <v>154.4</v>
       </c>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.35">
@@ -43765,7 +43773,7 @@
         <v>5798194.0027000001</v>
       </c>
       <c r="AB35">
-        <v>145.4</v>
+        <v>1833.4</v>
       </c>
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.35">
@@ -43925,7 +43933,7 @@
         <v>5799225.9619000005</v>
       </c>
       <c r="AB37">
-        <v>115.3</v>
+        <v>194.1</v>
       </c>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.35">
@@ -44005,7 +44013,7 @@
         <v>5799574.3284999998</v>
       </c>
       <c r="AB38">
-        <v>153.9</v>
+        <v>435.6</v>
       </c>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.35">
@@ -44165,7 +44173,7 @@
         <v>5800759.4974999996</v>
       </c>
       <c r="AB40">
-        <v>979.5</v>
+        <v>1802.9</v>
       </c>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.35">
@@ -44245,7 +44253,7 @@
         <v>5800881.9620000003</v>
       </c>
       <c r="AB41">
-        <v>32</v>
+        <v>193.1</v>
       </c>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.35">
@@ -44325,7 +44333,7 @@
         <v>5801438.6429000003</v>
       </c>
       <c r="AB42">
-        <v>98.1</v>
+        <v>427.70000000000005</v>
       </c>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.35">
@@ -44405,7 +44413,7 @@
         <v>5801629.6880000001</v>
       </c>
       <c r="AB43">
-        <v>2.5</v>
+        <v>196.39999999999998</v>
       </c>
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.35">
@@ -44485,7 +44493,7 @@
         <v>5802239.0274999999</v>
       </c>
       <c r="AB44">
-        <v>16.7</v>
+        <v>65.5</v>
       </c>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.35">
@@ -44565,7 +44573,7 @@
         <v>5802360.6118000001</v>
       </c>
       <c r="AB45">
-        <v>236.5</v>
+        <v>2960.6</v>
       </c>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.35">
@@ -44645,7 +44653,7 @@
         <v>5802769.2301000003</v>
       </c>
       <c r="AB46">
-        <v>2.2000000000000002</v>
+        <v>81.400000000000006</v>
       </c>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.35">
@@ -44725,7 +44733,7 @@
         <v>5802839.1476999996</v>
       </c>
       <c r="AB47">
-        <v>250.6</v>
+        <v>1320.7</v>
       </c>
     </row>
     <row r="48" spans="1:28" x14ac:dyDescent="0.35">
@@ -44805,7 +44813,7 @@
         <v>5802946.4726</v>
       </c>
       <c r="AB48">
-        <v>50.2</v>
+        <v>346.70000000000005</v>
       </c>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.35">
@@ -44885,7 +44893,7 @@
         <v>5803036.983</v>
       </c>
       <c r="AB49">
-        <v>125</v>
+        <v>483.7</v>
       </c>
     </row>
     <row r="50" spans="1:28" x14ac:dyDescent="0.35">
@@ -44965,7 +44973,7 @@
         <v>5803059.4765999997</v>
       </c>
       <c r="AB50">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="51" spans="1:28" x14ac:dyDescent="0.35">
@@ -45045,7 +45053,7 @@
         <v>5803476.9960000003</v>
       </c>
       <c r="AB51">
-        <v>1.3</v>
+        <v>260.70000000000005</v>
       </c>
     </row>
     <row r="52" spans="1:28" x14ac:dyDescent="0.35">
@@ -45125,7 +45133,7 @@
         <v>5803522.0323000001</v>
       </c>
       <c r="AB52">
-        <v>25.5</v>
+        <v>29.6</v>
       </c>
     </row>
     <row r="53" spans="1:28" x14ac:dyDescent="0.35">
@@ -45205,7 +45213,7 @@
         <v>5803599.9890000001</v>
       </c>
       <c r="AB53">
-        <v>3.3</v>
+        <v>2987.6</v>
       </c>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.35">
@@ -45285,7 +45293,7 @@
         <v>5803692.5104</v>
       </c>
       <c r="AB54">
-        <v>52.9</v>
+        <v>238.1</v>
       </c>
     </row>
     <row r="55" spans="1:28" x14ac:dyDescent="0.35">
@@ -45525,7 +45533,7 @@
         <v>5804633.8442000002</v>
       </c>
       <c r="AB57">
-        <v>0.4</v>
+        <v>35</v>
       </c>
     </row>
     <row r="58" spans="1:28" x14ac:dyDescent="0.35">
@@ -45605,7 +45613,7 @@
         <v>5804683.358</v>
       </c>
       <c r="AB58">
-        <v>183.1</v>
+        <v>868.50000000000011</v>
       </c>
     </row>
     <row r="59" spans="1:28" x14ac:dyDescent="0.35">
@@ -45685,7 +45693,7 @@
         <v>5804697.9941999996</v>
       </c>
       <c r="AB59">
-        <v>87.6</v>
+        <v>205.3</v>
       </c>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.35">
@@ -45845,7 +45853,7 @@
         <v>5805051.6851000004</v>
       </c>
       <c r="AB61">
-        <v>10.9</v>
+        <v>214.1</v>
       </c>
     </row>
     <row r="62" spans="1:28" x14ac:dyDescent="0.35">
@@ -46005,7 +46013,7 @@
         <v>5805911.9806000004</v>
       </c>
       <c r="AB63">
-        <v>267.39999999999998</v>
+        <v>534.79999999999995</v>
       </c>
     </row>
     <row r="64" spans="1:28" x14ac:dyDescent="0.35">
@@ -46085,7 +46093,7 @@
         <v>5805980.8996000001</v>
       </c>
       <c r="AB64">
-        <v>553.79999999999995</v>
+        <v>2764.4999999999995</v>
       </c>
     </row>
     <row r="65" spans="1:28" x14ac:dyDescent="0.35">
@@ -46165,7 +46173,7 @@
         <v>5805988.4506000001</v>
       </c>
       <c r="AB65">
-        <v>3.2</v>
+        <v>32.4</v>
       </c>
     </row>
     <row r="66" spans="1:28" x14ac:dyDescent="0.35">
@@ -46245,7 +46253,7 @@
         <v>5805995.0094999997</v>
       </c>
       <c r="AB66">
-        <v>8</v>
+        <v>1099.3999999999999</v>
       </c>
     </row>
     <row r="67" spans="1:28" x14ac:dyDescent="0.35">
@@ -46325,7 +46333,7 @@
         <v>5806249.5071</v>
       </c>
       <c r="AB67">
-        <v>52.4</v>
+        <v>83.9</v>
       </c>
     </row>
     <row r="68" spans="1:28" x14ac:dyDescent="0.35">
@@ -46405,7 +46413,7 @@
         <v>5806256.9930999996</v>
       </c>
       <c r="AB68">
-        <v>372.7</v>
+        <v>1372.1</v>
       </c>
     </row>
     <row r="69" spans="1:28" x14ac:dyDescent="0.35">
@@ -46485,7 +46493,7 @@
         <v>5806263.0338000003</v>
       </c>
       <c r="AB69">
-        <v>122</v>
+        <v>216</v>
       </c>
     </row>
     <row r="70" spans="1:28" x14ac:dyDescent="0.35">
@@ -46565,7 +46573,7 @@
         <v>5806324.5248999996</v>
       </c>
       <c r="AB70">
-        <v>314.2</v>
+        <v>573.29999999999995</v>
       </c>
     </row>
     <row r="71" spans="1:28" x14ac:dyDescent="0.35">
@@ -46805,7 +46813,7 @@
         <v>5806571.4941999996</v>
       </c>
       <c r="AB73">
-        <v>0</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="74" spans="1:28" x14ac:dyDescent="0.35">
@@ -46885,7 +46893,7 @@
         <v>5806572.4687000001</v>
       </c>
       <c r="AB74">
-        <v>57.5</v>
+        <v>77</v>
       </c>
     </row>
     <row r="75" spans="1:28" x14ac:dyDescent="0.35">
@@ -46965,7 +46973,7 @@
         <v>5806619.9822000004</v>
       </c>
       <c r="AB75">
-        <v>34.799999999999997</v>
+        <v>125.89999999999999</v>
       </c>
     </row>
     <row r="76" spans="1:28" x14ac:dyDescent="0.35">
@@ -47045,7 +47053,7 @@
         <v>5806709.9983000001</v>
       </c>
       <c r="AB76">
-        <v>118.1</v>
+        <v>118.8</v>
       </c>
     </row>
     <row r="77" spans="1:28" x14ac:dyDescent="0.35">
@@ -47125,7 +47133,7 @@
         <v>5806886.5061999997</v>
       </c>
       <c r="AB77">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:28" x14ac:dyDescent="0.35">
@@ -47205,7 +47213,7 @@
         <v>5806915.5203999998</v>
       </c>
       <c r="AB78">
-        <v>0.7</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="79" spans="1:28" x14ac:dyDescent="0.35">
@@ -47285,7 +47293,7 @@
         <v>5806973.0005999999</v>
       </c>
       <c r="AB79">
-        <v>26.6</v>
+        <v>34.300000000000004</v>
       </c>
     </row>
     <row r="80" spans="1:28" x14ac:dyDescent="0.35">
@@ -47445,7 +47453,7 @@
         <v>5807873.5072999997</v>
       </c>
       <c r="AB81">
-        <v>8.4</v>
+        <v>24.3</v>
       </c>
     </row>
     <row r="82" spans="1:28" x14ac:dyDescent="0.35">
@@ -47525,7 +47533,7 @@
         <v>5808009.4837999996</v>
       </c>
       <c r="AB82">
-        <v>154.6</v>
+        <v>251.7</v>
       </c>
     </row>
     <row r="83" spans="1:28" x14ac:dyDescent="0.35">
@@ -47605,7 +47613,7 @@
         <v>5808173.4556999998</v>
       </c>
       <c r="AB83">
-        <v>10.4</v>
+        <v>12.600000000000001</v>
       </c>
     </row>
     <row r="84" spans="1:28" x14ac:dyDescent="0.35">
@@ -47685,7 +47693,7 @@
         <v>5808292.9885999998</v>
       </c>
       <c r="AB84">
-        <v>88.2</v>
+        <v>462.79999999999995</v>
       </c>
     </row>
     <row r="85" spans="1:28" x14ac:dyDescent="0.35">
@@ -47765,7 +47773,7 @@
         <v>5808364.4950000001</v>
       </c>
       <c r="AB85">
-        <v>6.3</v>
+        <v>22.2</v>
       </c>
     </row>
     <row r="86" spans="1:28" x14ac:dyDescent="0.35">
@@ -47845,7 +47853,7 @@
         <v>5808909.9967999998</v>
       </c>
       <c r="AB86">
-        <v>6.9</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="87" spans="1:28" x14ac:dyDescent="0.35">
@@ -47925,7 +47933,7 @@
         <v>5808960.9755999995</v>
       </c>
       <c r="AB87">
-        <v>16.3</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="88" spans="1:28" x14ac:dyDescent="0.35">
@@ -48005,7 +48013,7 @@
         <v>5809570.6155000003</v>
       </c>
       <c r="AB88">
-        <v>121.2</v>
+        <v>373.9</v>
       </c>
     </row>
     <row r="89" spans="1:28" x14ac:dyDescent="0.35">
@@ -48085,7 +48093,7 @@
         <v>5810307.3421</v>
       </c>
       <c r="AB89">
-        <v>5.6</v>
+        <v>155.6</v>
       </c>
     </row>
     <row r="90" spans="1:28" x14ac:dyDescent="0.35">
@@ -48405,7 +48413,7 @@
         <v>5811953.2414999995</v>
       </c>
       <c r="AB93">
-        <v>11.5</v>
+        <v>34.699999999999996</v>
       </c>
     </row>
     <row r="94" spans="1:28" x14ac:dyDescent="0.35">
@@ -48485,7 +48493,7 @@
         <v>5812026.4763000002</v>
       </c>
       <c r="AB94">
-        <v>1.1000000000000001</v>
+        <v>30.1</v>
       </c>
     </row>
     <row r="95" spans="1:28" x14ac:dyDescent="0.35">
@@ -48565,7 +48573,7 @@
         <v>5812111.9911000002</v>
       </c>
       <c r="AB95">
-        <v>21.8</v>
+        <v>68.400000000000006</v>
       </c>
     </row>
     <row r="96" spans="1:28" x14ac:dyDescent="0.35">
@@ -48725,7 +48733,7 @@
         <v>5812474.4885999998</v>
       </c>
       <c r="AB97">
-        <v>18.8</v>
+        <v>160.5</v>
       </c>
     </row>
     <row r="98" spans="1:28" x14ac:dyDescent="0.35">
@@ -48805,7 +48813,7 @@
         <v>5812517.1518000001</v>
       </c>
       <c r="AB98">
-        <v>567.20000000000005</v>
+        <v>1529.0000000000002</v>
       </c>
     </row>
     <row r="99" spans="1:28" x14ac:dyDescent="0.35">
@@ -48885,7 +48893,7 @@
         <v>5812530.6333999997</v>
       </c>
       <c r="AB99">
-        <v>415</v>
+        <v>5851.3</v>
       </c>
     </row>
     <row r="100" spans="1:28" x14ac:dyDescent="0.35">
@@ -48965,7 +48973,7 @@
         <v>5812549.9899000004</v>
       </c>
       <c r="AB100">
-        <v>214.6</v>
+        <v>917.3</v>
       </c>
     </row>
     <row r="101" spans="1:28" x14ac:dyDescent="0.35">
@@ -49044,8 +49052,8 @@
       <c r="AA101">
         <v>5812730.0321000004</v>
       </c>
-      <c r="AB101" t="e">
-        <v>#N/A</v>
+      <c r="AB101">
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:28" x14ac:dyDescent="0.35">
@@ -49125,7 +49133,7 @@
         <v>5812800.5064000003</v>
       </c>
       <c r="AB102">
-        <v>52.6</v>
+        <v>56.5</v>
       </c>
     </row>
     <row r="103" spans="1:28" x14ac:dyDescent="0.35">
@@ -49205,7 +49213,7 @@
         <v>5812816.9682</v>
       </c>
       <c r="AB103">
-        <v>139.30000000000001</v>
+        <v>142</v>
       </c>
     </row>
     <row r="104" spans="1:28" x14ac:dyDescent="0.35">
@@ -49285,7 +49293,7 @@
         <v>5812818.8477999996</v>
       </c>
       <c r="AB104">
-        <v>22.5</v>
+        <v>880.3</v>
       </c>
     </row>
     <row r="105" spans="1:28" x14ac:dyDescent="0.35">
@@ -49365,7 +49373,7 @@
         <v>5813204.0237999996</v>
       </c>
       <c r="AB105">
-        <v>218.8</v>
+        <v>1926.1</v>
       </c>
     </row>
     <row r="106" spans="1:28" x14ac:dyDescent="0.35">
@@ -49445,7 +49453,7 @@
         <v>5813314.5256000003</v>
       </c>
       <c r="AB106">
-        <v>11.6</v>
+        <v>115.8</v>
       </c>
     </row>
     <row r="107" spans="1:28" x14ac:dyDescent="0.35">
@@ -49525,7 +49533,7 @@
         <v>5813582.4753</v>
       </c>
       <c r="AB107">
-        <v>9.6999999999999993</v>
+        <v>30.2</v>
       </c>
     </row>
     <row r="108" spans="1:28" x14ac:dyDescent="0.35">
@@ -49605,7 +49613,7 @@
         <v>5813618.4955000002</v>
       </c>
       <c r="AB108">
-        <v>81.3</v>
+        <v>1679.6</v>
       </c>
     </row>
     <row r="109" spans="1:28" x14ac:dyDescent="0.35">
@@ -49765,7 +49773,7 @@
         <v>5813886.0224000001</v>
       </c>
       <c r="AB110">
-        <v>6.7</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="111" spans="1:28" x14ac:dyDescent="0.35">
@@ -49845,7 +49853,7 @@
         <v>5813946.4921000004</v>
       </c>
       <c r="AB111">
-        <v>7.4</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="112" spans="1:28" x14ac:dyDescent="0.35">
@@ -49925,7 +49933,7 @@
         <v>5813979.4978</v>
       </c>
       <c r="AB112">
-        <v>159.80000000000001</v>
+        <v>267.8</v>
       </c>
     </row>
     <row r="113" spans="1:28" x14ac:dyDescent="0.35">
@@ -50005,7 +50013,7 @@
         <v>5813988.0088</v>
       </c>
       <c r="AB113">
-        <v>5.8</v>
+        <v>69.8</v>
       </c>
     </row>
     <row r="114" spans="1:28" x14ac:dyDescent="0.35">
@@ -50085,7 +50093,7 @@
         <v>5814492.2026000004</v>
       </c>
       <c r="AB114">
-        <v>239.7</v>
+        <v>1186.0999999999999</v>
       </c>
     </row>
     <row r="115" spans="1:28" x14ac:dyDescent="0.35">
@@ -50165,7 +50173,7 @@
         <v>5814908.0252</v>
       </c>
       <c r="AB115">
-        <v>23.1</v>
+        <v>43.7</v>
       </c>
     </row>
     <row r="116" spans="1:28" x14ac:dyDescent="0.35">
@@ -50245,7 +50253,7 @@
         <v>5814975.5071999999</v>
       </c>
       <c r="AB116">
-        <v>72.3</v>
+        <v>192.39999999999998</v>
       </c>
     </row>
     <row r="117" spans="1:28" x14ac:dyDescent="0.35">
@@ -50325,7 +50333,7 @@
         <v>5815431.3154999996</v>
       </c>
       <c r="AB117">
-        <v>38.1</v>
+        <v>1240.2</v>
       </c>
     </row>
     <row r="118" spans="1:28" x14ac:dyDescent="0.35">
@@ -50405,7 +50413,7 @@
         <v>5815531.4627999999</v>
       </c>
       <c r="AB118">
-        <v>0.8</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="119" spans="1:28" x14ac:dyDescent="0.35">
@@ -50485,7 +50493,7 @@
         <v>5815581.0721000005</v>
       </c>
       <c r="AB119">
-        <v>14.5</v>
+        <v>2049.8000000000002</v>
       </c>
     </row>
     <row r="120" spans="1:28" x14ac:dyDescent="0.35">
@@ -50645,7 +50653,7 @@
         <v>5815745.0196000002</v>
       </c>
       <c r="AB121">
-        <v>37.700000000000003</v>
+        <v>90.8</v>
       </c>
     </row>
     <row r="122" spans="1:28" x14ac:dyDescent="0.35">
@@ -50725,7 +50733,7 @@
         <v>5816333.0016000001</v>
       </c>
       <c r="AB122">
-        <v>0.6</v>
+        <v>28.5</v>
       </c>
     </row>
     <row r="123" spans="1:28" x14ac:dyDescent="0.35">
@@ -50805,7 +50813,7 @@
         <v>5816546.0193999996</v>
       </c>
       <c r="AB123">
-        <v>1.5</v>
+        <v>21.4</v>
       </c>
     </row>
     <row r="124" spans="1:28" x14ac:dyDescent="0.35">
@@ -50885,7 +50893,7 @@
         <v>5816552.9501</v>
       </c>
       <c r="AB124">
-        <v>11.4</v>
+        <v>23.6</v>
       </c>
     </row>
     <row r="125" spans="1:28" x14ac:dyDescent="0.35">
@@ -50965,7 +50973,7 @@
         <v>5816706.9835000001</v>
       </c>
       <c r="AB125">
-        <v>186.5</v>
+        <v>373</v>
       </c>
     </row>
     <row r="126" spans="1:28" x14ac:dyDescent="0.35">
@@ -51045,7 +51053,7 @@
         <v>5816748.9721999997</v>
       </c>
       <c r="AB126">
-        <v>0</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="127" spans="1:28" x14ac:dyDescent="0.35">
@@ -51125,7 +51133,7 @@
         <v>5816865.0505999997</v>
       </c>
       <c r="AB127">
-        <v>18.8</v>
+        <v>120.3</v>
       </c>
     </row>
     <row r="128" spans="1:28" x14ac:dyDescent="0.35">
@@ -51285,7 +51293,7 @@
         <v>5817025.4989999998</v>
       </c>
       <c r="AB129">
-        <v>69</v>
+        <v>71.7</v>
       </c>
     </row>
     <row r="130" spans="1:28" x14ac:dyDescent="0.35">
@@ -51365,7 +51373,7 @@
         <v>5817353.4616999999</v>
       </c>
       <c r="AB130">
-        <v>8.1</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="131" spans="1:28" x14ac:dyDescent="0.35">
@@ -51605,7 +51613,7 @@
         <v>5818003.4972000001</v>
       </c>
       <c r="AB133">
-        <v>2.9</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="134" spans="1:28" x14ac:dyDescent="0.35">
@@ -51685,7 +51693,7 @@
         <v>5818030.6733999997</v>
       </c>
       <c r="AB134">
-        <v>62.4</v>
+        <v>367.8</v>
       </c>
     </row>
     <row r="135" spans="1:28" x14ac:dyDescent="0.35">
@@ -51765,7 +51773,7 @@
         <v>5818098.5384</v>
       </c>
       <c r="AB135">
-        <v>20.399999999999999</v>
+        <v>45.5</v>
       </c>
     </row>
     <row r="136" spans="1:28" x14ac:dyDescent="0.35">
@@ -52005,7 +52013,7 @@
         <v>5818764.9759999998</v>
       </c>
       <c r="AB138">
-        <v>19.8</v>
+        <v>35.4</v>
       </c>
     </row>
     <row r="139" spans="1:28" x14ac:dyDescent="0.35">
@@ -52085,7 +52093,7 @@
         <v>5818793.4605</v>
       </c>
       <c r="AB139">
-        <v>5.0999999999999996</v>
+        <v>28.5</v>
       </c>
     </row>
     <row r="140" spans="1:28" x14ac:dyDescent="0.35">
@@ -52244,8 +52252,8 @@
       <c r="AA141">
         <v>5819206.3502000002</v>
       </c>
-      <c r="AB141" t="e">
-        <v>#N/A</v>
+      <c r="AB141">
+        <v>348.5</v>
       </c>
     </row>
     <row r="142" spans="1:28" x14ac:dyDescent="0.35">
@@ -52325,7 +52333,7 @@
         <v>5819347.2598000001</v>
       </c>
       <c r="AB142">
-        <v>161.5</v>
+        <v>560.29999999999995</v>
       </c>
     </row>
     <row r="143" spans="1:28" x14ac:dyDescent="0.35">
@@ -52405,7 +52413,7 @@
         <v>5819400.9863999998</v>
       </c>
       <c r="AB143">
-        <v>20.6</v>
+        <v>39</v>
       </c>
     </row>
     <row r="144" spans="1:28" x14ac:dyDescent="0.35">
@@ -52485,7 +52493,7 @@
         <v>5819923.1506000003</v>
       </c>
       <c r="AB144">
-        <v>67.2</v>
+        <v>856.60000000000014</v>
       </c>
     </row>
     <row r="145" spans="1:28" x14ac:dyDescent="0.35">
@@ -52565,7 +52573,7 @@
         <v>5820248.4051000001</v>
       </c>
       <c r="AB145">
-        <v>117.6</v>
+        <v>692.9</v>
       </c>
     </row>
     <row r="146" spans="1:28" x14ac:dyDescent="0.35">
@@ -52645,7 +52653,7 @@
         <v>5820616.0237999996</v>
       </c>
       <c r="AB146">
-        <v>0.4</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="147" spans="1:28" x14ac:dyDescent="0.35">
@@ -52805,7 +52813,7 @@
         <v>5820943.4989</v>
       </c>
       <c r="AB148">
-        <v>50.6</v>
+        <v>91.4</v>
       </c>
     </row>
     <row r="149" spans="1:28" x14ac:dyDescent="0.35">
@@ -52885,7 +52893,7 @@
         <v>5820971.4726999998</v>
       </c>
       <c r="AB149">
-        <v>280</v>
+        <v>442.5</v>
       </c>
     </row>
     <row r="150" spans="1:28" x14ac:dyDescent="0.35">
@@ -52965,7 +52973,7 @@
         <v>5821406.5033999998</v>
       </c>
       <c r="AB150">
-        <v>206.8</v>
+        <v>439.6</v>
       </c>
     </row>
     <row r="151" spans="1:28" x14ac:dyDescent="0.35">
@@ -53045,7 +53053,7 @@
         <v>5821770.4901000001</v>
       </c>
       <c r="AB151">
-        <v>10.199999999999999</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="152" spans="1:28" x14ac:dyDescent="0.35">
@@ -53125,7 +53133,7 @@
         <v>5821843.0312000001</v>
       </c>
       <c r="AB152">
-        <v>118.9</v>
+        <v>150.1</v>
       </c>
     </row>
     <row r="153" spans="1:28" x14ac:dyDescent="0.35">
@@ -53365,7 +53373,7 @@
         <v>5822797.9863</v>
       </c>
       <c r="AB155">
-        <v>152.19999999999999</v>
+        <v>158.5</v>
       </c>
     </row>
     <row r="156" spans="1:28" x14ac:dyDescent="0.35">
@@ -53445,7 +53453,7 @@
         <v>5823179.5405999999</v>
       </c>
       <c r="AB156">
-        <v>39</v>
+        <v>50.6</v>
       </c>
     </row>
     <row r="157" spans="1:28" x14ac:dyDescent="0.35">
@@ -53524,8 +53532,8 @@
       <c r="AA157">
         <v>5823732.2582999999</v>
       </c>
-      <c r="AB157" t="e">
-        <v>#N/A</v>
+      <c r="AB157">
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:28" x14ac:dyDescent="0.35">
@@ -53605,7 +53613,7 @@
         <v>5823802.9973999998</v>
       </c>
       <c r="AB158">
-        <v>94.5</v>
+        <v>122.7</v>
       </c>
     </row>
     <row r="159" spans="1:28" x14ac:dyDescent="0.35">
@@ -53765,7 +53773,7 @@
         <v>5824401.4228999997</v>
       </c>
       <c r="AB160">
-        <v>11.5</v>
+        <v>302.5</v>
       </c>
     </row>
     <row r="161" spans="1:28" x14ac:dyDescent="0.35">
@@ -53925,7 +53933,7 @@
         <v>5824603.4926000005</v>
       </c>
       <c r="AB162">
-        <v>30.5</v>
+        <v>66.2</v>
       </c>
     </row>
     <row r="163" spans="1:28" x14ac:dyDescent="0.35">
@@ -54005,7 +54013,7 @@
         <v>5824779.0406999998</v>
       </c>
       <c r="AB163">
-        <v>6.3</v>
+        <v>14.8</v>
       </c>
     </row>
     <row r="164" spans="1:28" x14ac:dyDescent="0.35">
@@ -54085,7 +54093,7 @@
         <v>5824920.6321999999</v>
       </c>
       <c r="AB164">
-        <v>125.5</v>
+        <v>500.8</v>
       </c>
     </row>
     <row r="165" spans="1:28" x14ac:dyDescent="0.35">
@@ -54165,7 +54173,7 @@
         <v>5825058.6242000004</v>
       </c>
       <c r="AB165">
-        <v>92.5</v>
+        <v>880.3</v>
       </c>
     </row>
     <row r="166" spans="1:28" x14ac:dyDescent="0.35">
@@ -54325,7 +54333,7 @@
         <v>5825400.3409000002</v>
       </c>
       <c r="AB167">
-        <v>135.4</v>
+        <v>600.9</v>
       </c>
     </row>
     <row r="168" spans="1:28" x14ac:dyDescent="0.35">
@@ -54405,7 +54413,7 @@
         <v>5825436.9919999996</v>
       </c>
       <c r="AB168">
-        <v>8</v>
+        <v>28.099999999999998</v>
       </c>
     </row>
     <row r="169" spans="1:28" x14ac:dyDescent="0.35">
@@ -54485,7 +54493,7 @@
         <v>5825485.5136000002</v>
       </c>
       <c r="AB169">
-        <v>71</v>
+        <v>71.099999999999994</v>
       </c>
     </row>
     <row r="170" spans="1:28" x14ac:dyDescent="0.35">
@@ -54565,7 +54573,7 @@
         <v>5826165.4855000004</v>
       </c>
       <c r="AB170">
-        <v>160.6</v>
+        <v>306.7</v>
       </c>
     </row>
     <row r="171" spans="1:28" x14ac:dyDescent="0.35">
@@ -54725,7 +54733,7 @@
         <v>5827290.9137000004</v>
       </c>
       <c r="AB172">
-        <v>40.1</v>
+        <v>736.5</v>
       </c>
     </row>
     <row r="173" spans="1:28" x14ac:dyDescent="0.35">
@@ -54805,7 +54813,7 @@
         <v>5827769.375</v>
       </c>
       <c r="AB173">
-        <v>56.3</v>
+        <v>587.70000000000005</v>
       </c>
     </row>
     <row r="174" spans="1:28" x14ac:dyDescent="0.35">
@@ -54885,7 +54893,7 @@
         <v>5828726.0362</v>
       </c>
       <c r="AB174">
-        <v>21.7</v>
+        <v>23.3</v>
       </c>
     </row>
     <row r="175" spans="1:28" x14ac:dyDescent="0.35">
@@ -54965,7 +54973,7 @@
         <v>5828847.0066</v>
       </c>
       <c r="AB175">
-        <v>10.199999999999999</v>
+        <v>58.099999999999994</v>
       </c>
     </row>
     <row r="176" spans="1:28" x14ac:dyDescent="0.35">
@@ -55045,7 +55053,7 @@
         <v>5829216.9916000003</v>
       </c>
       <c r="AB176">
-        <v>39.9</v>
+        <v>208.5</v>
       </c>
     </row>
     <row r="177" spans="1:28" x14ac:dyDescent="0.35">
@@ -55125,7 +55133,7 @@
         <v>5829381.3509999998</v>
       </c>
       <c r="AB177">
-        <v>6.4</v>
+        <v>65.599999999999994</v>
       </c>
     </row>
     <row r="178" spans="1:28" x14ac:dyDescent="0.35">
@@ -55205,7 +55213,7 @@
         <v>5829491.4731000001</v>
       </c>
       <c r="AB178">
-        <v>4.7</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="179" spans="1:28" x14ac:dyDescent="0.35">
@@ -55285,7 +55293,7 @@
         <v>5829686.9617999997</v>
       </c>
       <c r="AB179">
-        <v>1.1000000000000001</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="180" spans="1:28" x14ac:dyDescent="0.35">
@@ -55365,7 +55373,7 @@
         <v>5829830.0143999998</v>
       </c>
       <c r="AB180">
-        <v>11.2</v>
+        <v>21.2</v>
       </c>
     </row>
     <row r="181" spans="1:28" x14ac:dyDescent="0.35">
@@ -55445,7 +55453,7 @@
         <v>5829882.0060000001</v>
       </c>
       <c r="AB181">
-        <v>20.5</v>
+        <v>25.7</v>
       </c>
     </row>
     <row r="182" spans="1:28" x14ac:dyDescent="0.35">
@@ -55525,7 +55533,7 @@
         <v>5829916.5427999999</v>
       </c>
       <c r="AB182">
-        <v>1</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="183" spans="1:28" x14ac:dyDescent="0.35">
@@ -55605,7 +55613,7 @@
         <v>5830921.2950999998</v>
       </c>
       <c r="AB183">
-        <v>3.8</v>
+        <v>760.2</v>
       </c>
     </row>
     <row r="184" spans="1:28" x14ac:dyDescent="0.35">
@@ -55685,7 +55693,7 @@
         <v>5831325.3553999998</v>
       </c>
       <c r="AB184">
-        <v>65.3</v>
+        <v>857.49999999999989</v>
       </c>
     </row>
     <row r="185" spans="1:28" x14ac:dyDescent="0.35">
@@ -55765,7 +55773,7 @@
         <v>5832262.5869000005</v>
       </c>
       <c r="AB185">
-        <v>117.7</v>
+        <v>252.10000000000002</v>
       </c>
     </row>
     <row r="186" spans="1:28" x14ac:dyDescent="0.35">
@@ -55845,7 +55853,7 @@
         <v>5833072.5148999998</v>
       </c>
       <c r="AB186">
-        <v>4.3</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="187" spans="1:28" x14ac:dyDescent="0.35">
@@ -56005,7 +56013,7 @@
         <v>5834306.5016999999</v>
       </c>
       <c r="AB188">
-        <v>1.8</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="189" spans="1:28" x14ac:dyDescent="0.35">
@@ -56085,7 +56093,7 @@
         <v>5834355.9748999998</v>
       </c>
       <c r="AB189">
-        <v>2.6</v>
+        <v>10.3</v>
       </c>
     </row>
     <row r="190" spans="1:28" x14ac:dyDescent="0.35">
@@ -56245,7 +56253,7 @@
         <v>5836615.2604999999</v>
       </c>
       <c r="AB191">
-        <v>33</v>
+        <v>242.5</v>
       </c>
     </row>
     <row r="192" spans="1:28" x14ac:dyDescent="0.35">
@@ -56325,10 +56333,11 @@
         <v>5838486.4243000001</v>
       </c>
       <c r="AB192">
-        <v>76.599999999999994</v>
+        <v>853.8</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AB192" xr:uid="{A0BFFBAD-06FD-491E-9425-0183DA3A5D3D}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>